<commit_message>
Fix upper bound of EE std policy for cooling building components
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -31789,9 +31789,6 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -31800,6 +31797,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -31827,17 +31827,7 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Обычный_CRF2002 (1)" xfId="13"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -32916,9 +32906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T553"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -40542,7 +40532,7 @@
         <v>0</v>
       </c>
       <c r="M132" s="63">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="N132" s="61">
         <v>0.01</v>
@@ -40908,7 +40898,7 @@
         <v>0</v>
       </c>
       <c r="M138" s="61">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="N138" s="61">
         <v>0.01</v>
@@ -41280,7 +41270,7 @@
         <v>0</v>
       </c>
       <c r="M144" s="61">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="N144" s="61">
         <v>0.01</v>
@@ -63541,42 +63531,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I76:I88 I518 I520:I539 I541:I1048576 I90:I99 I1:I9 I12:I19 I24 I33:I36 I43:I46 I53:I59 I38:I39 I48:I49 I63:I64 I312:I317 I322:I327 I332:I337 I352:I353 I362:I367 I342:I350 I355 I357 I113:I307 I372:I483 I485:I516">
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I519">
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I519)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66 I74 I22 I32 I42 I52">
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65">
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67:I73">
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I89">
-    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I484">
-    <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I484)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -64438,7 +64428,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="30">
       <c r="A30" s="157" t="s">
         <v>2718</v>
       </c>
@@ -81784,13 +81774,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="268" t="s">
+      <c r="A1" s="271" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="268"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="272" t="s">
@@ -81859,13 +81849,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="268" t="s">
+      <c r="A60" s="271" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="268"/>
-      <c r="C60" s="268"/>
-      <c r="D60" s="268"/>
-      <c r="E60" s="268"/>
+      <c r="B60" s="271"/>
+      <c r="C60" s="271"/>
+      <c r="D60" s="271"/>
+      <c r="E60" s="271"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1">
       <c r="A85" s="11" t="s">
@@ -81970,13 +81960,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="268" t="s">
+      <c r="A89" s="271" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="268"/>
-      <c r="C89" s="268"/>
-      <c r="D89" s="268"/>
-      <c r="E89" s="268"/>
+      <c r="B89" s="271"/>
+      <c r="C89" s="271"/>
+      <c r="D89" s="271"/>
+      <c r="E89" s="271"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="11">
@@ -82063,13 +82053,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="268" t="s">
+      <c r="A98" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="268"/>
-      <c r="C98" s="268"/>
-      <c r="D98" s="268"/>
-      <c r="E98" s="268"/>
+      <c r="B98" s="271"/>
+      <c r="C98" s="271"/>
+      <c r="D98" s="271"/>
+      <c r="E98" s="271"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="19">
@@ -82153,13 +82143,13 @@
       <c r="A108" s="22"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="268" t="s">
+      <c r="A109" s="271" t="s">
         <v>187</v>
       </c>
-      <c r="B109" s="268"/>
-      <c r="C109" s="268"/>
-      <c r="D109" s="268"/>
-      <c r="E109" s="268"/>
+      <c r="B109" s="271"/>
+      <c r="C109" s="271"/>
+      <c r="D109" s="271"/>
+      <c r="E109" s="271"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1">
@@ -82172,13 +82162,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="268" t="s">
+      <c r="A113" s="271" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="268"/>
-      <c r="C113" s="268"/>
-      <c r="D113" s="268"/>
-      <c r="E113" s="268"/>
+      <c r="B113" s="271"/>
+      <c r="C113" s="271"/>
+      <c r="D113" s="271"/>
+      <c r="E113" s="271"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="19">
@@ -82259,13 +82249,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="268" t="s">
+      <c r="A124" s="271" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="268"/>
-      <c r="C124" s="268"/>
-      <c r="D124" s="268"/>
-      <c r="E124" s="268"/>
+      <c r="B124" s="271"/>
+      <c r="C124" s="271"/>
+      <c r="D124" s="271"/>
+      <c r="E124" s="271"/>
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:14">
@@ -82356,13 +82346,13 @@
       <c r="C133" s="17"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="268" t="s">
+      <c r="A134" s="271" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="268"/>
-      <c r="C134" s="268"/>
-      <c r="D134" s="268"/>
-      <c r="E134" s="268"/>
+      <c r="B134" s="271"/>
+      <c r="C134" s="271"/>
+      <c r="D134" s="271"/>
+      <c r="E134" s="271"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="29" t="s">
@@ -82377,25 +82367,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75">
       <c r="A136" s="31"/>
-      <c r="B136" s="269" t="s">
+      <c r="B136" s="268" t="s">
         <v>469</v>
       </c>
-      <c r="C136" s="270"/>
-      <c r="D136" s="270"/>
-      <c r="E136" s="271"/>
+      <c r="C136" s="269"/>
+      <c r="D136" s="269"/>
+      <c r="E136" s="270"/>
       <c r="F136" s="30"/>
       <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:14" ht="15.75">
       <c r="A137" s="32"/>
-      <c r="B137" s="269" t="s">
+      <c r="B137" s="268" t="s">
         <v>470</v>
       </c>
-      <c r="C137" s="271"/>
-      <c r="D137" s="269" t="s">
+      <c r="C137" s="270"/>
+      <c r="D137" s="268" t="s">
         <v>471</v>
       </c>
-      <c r="E137" s="271"/>
+      <c r="E137" s="270"/>
       <c r="F137" s="30"/>
       <c r="G137" s="30"/>
     </row>
@@ -82942,13 +82932,13 @@
       <c r="G163" s="30"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="268" t="s">
+      <c r="A165" s="271" t="s">
         <v>190</v>
       </c>
-      <c r="B165" s="268"/>
-      <c r="C165" s="268"/>
-      <c r="D165" s="268"/>
-      <c r="E165" s="268"/>
+      <c r="B165" s="271"/>
+      <c r="C165" s="271"/>
+      <c r="D165" s="271"/>
+      <c r="E165" s="271"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1">
       <c r="A166" s="25" t="s">
@@ -82971,10 +82961,10 @@
       <c r="B168" s="48"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="268" t="s">
+      <c r="A169" s="271" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="268"/>
+      <c r="B169" s="271"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="25" t="s">
@@ -83006,13 +82996,13 @@
       <c r="B173" s="48"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="268" t="s">
+      <c r="A174" s="271" t="s">
         <v>199</v>
       </c>
-      <c r="B174" s="268"/>
-      <c r="C174" s="268"/>
-      <c r="D174" s="268"/>
-      <c r="E174" s="268"/>
+      <c r="B174" s="271"/>
+      <c r="C174" s="271"/>
+      <c r="D174" s="271"/>
+      <c r="E174" s="271"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1">
       <c r="A175" s="25" t="s">
@@ -83032,13 +83022,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="268" t="s">
+      <c r="A178" s="271" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="268"/>
-      <c r="C178" s="268"/>
-      <c r="D178" s="268"/>
-      <c r="E178" s="268"/>
+      <c r="B178" s="271"/>
+      <c r="C178" s="271"/>
+      <c r="D178" s="271"/>
+      <c r="E178" s="271"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="27" t="s">
@@ -83066,13 +83056,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="268" t="s">
+      <c r="A183" s="271" t="s">
         <v>195</v>
       </c>
-      <c r="B183" s="268"/>
-      <c r="C183" s="268"/>
-      <c r="D183" s="268"/>
-      <c r="E183" s="268"/>
+      <c r="B183" s="271"/>
+      <c r="C183" s="271"/>
+      <c r="D183" s="271"/>
+      <c r="E183" s="271"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="25" t="s">
@@ -83127,13 +83117,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="268" t="s">
+      <c r="A191" s="271" t="s">
         <v>209</v>
       </c>
-      <c r="B191" s="268"/>
-      <c r="C191" s="268"/>
-      <c r="D191" s="268"/>
-      <c r="E191" s="268"/>
+      <c r="B191" s="271"/>
+      <c r="C191" s="271"/>
+      <c r="D191" s="271"/>
+      <c r="E191" s="271"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="23" t="s">
@@ -83193,6 +83183,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -83207,12 +83203,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -83221,21 +83211,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -83473,14 +83463,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -83494,6 +83476,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Rename BAU scenario "Existing Policies"
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -28955,9 +28955,6 @@
     <t>https://www.energypolicy.solutions</t>
   </si>
   <si>
-    <t>Current Policy Scenario</t>
-  </si>
-  <si>
     <t>**Description:** This policy represents strengthening standards for VOCs emitted by aircraft.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Hong Kong, road transport was a major emission source of NOx, VOC and CO, accounting for 20%, 19% and 53% of the total emissions in 2017, respectively.  Overall, the emissions from road transport decreased by 45% to 98% from 2001 to 2017, despite an increase in vehicle-kilometer-travelled of 19% during the same period</t>
   </si>
   <si>
@@ -29997,6 +29994,9 @@
   </si>
   <si>
     <t>**Description:** This policy causes the capital cost of hydrogen vehicles to decline by the set percentage over the course of the model run.  The R&amp;D progress caused by this policy is additional to any R&amp;D necessary to comply with other policies, such as tighter fuel economy standards.  No costs associated with conducting this additional R&amp;D (such as investments in laboratories or engineers' salaries) are included in the model. // **Guidance for setting values:** This policy should generally be set to zero unless you are exploring a scenario with unusual and unexpected technological advancement.  If setting a non-zero value, more mature technologies, such as coal, should have lower values than younger technologies, such as solar.  A setting of 30% implies an average of roughly 1% annual improvement, which is very substantial.</t>
+  </si>
+  <si>
+    <t>Existing Policies</t>
   </si>
 </sst>
 </file>
@@ -31789,6 +31789,9 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -31797,9 +31800,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -32817,7 +32817,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -32906,7 +32906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A141" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A144" sqref="A144"/>
     </sheetView>
@@ -33042,7 +33042,7 @@
         <v>2221</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>2223</v>
@@ -33051,7 +33051,7 @@
         <v>2222</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T2" s="3">
         <v>0</v>
@@ -33104,7 +33104,7 @@
         <v>2221</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>2223</v>
@@ -33113,7 +33113,7 @@
         <v>2222</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T3" s="3">
         <v>0</v>
@@ -33166,7 +33166,7 @@
         <v>2221</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>2223</v>
@@ -33175,7 +33175,7 @@
         <v>2222</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T4" s="3">
         <v>0</v>
@@ -33228,7 +33228,7 @@
         <v>2221</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>2223</v>
@@ -33237,7 +33237,7 @@
         <v>2222</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T5" s="3">
         <v>0</v>
@@ -33290,7 +33290,7 @@
         <v>2221</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>2223</v>
@@ -33299,7 +33299,7 @@
         <v>2222</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T6" s="3">
         <v>0</v>
@@ -33352,7 +33352,7 @@
         <v>2221</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>2223</v>
@@ -33361,7 +33361,7 @@
         <v>2222</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T7" s="3">
         <v>0</v>
@@ -33414,7 +33414,7 @@
         <v>2221</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>2223</v>
@@ -33423,7 +33423,7 @@
         <v>2222</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T8" s="3">
         <v>0</v>
@@ -33476,7 +33476,7 @@
         <v>2221</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>2223</v>
@@ -33485,7 +33485,7 @@
         <v>2222</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T9" s="3">
         <v>0</v>
@@ -33638,7 +33638,7 @@
         <v>2221</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>2223</v>
@@ -33647,7 +33647,7 @@
         <v>2222</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T12" s="3">
         <v>0</v>
@@ -33700,7 +33700,7 @@
         <v>2221</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>2223</v>
@@ -33709,7 +33709,7 @@
         <v>2222</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T13" s="3">
         <v>0</v>
@@ -33762,7 +33762,7 @@
         <v>2221</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>2223</v>
@@ -33771,7 +33771,7 @@
         <v>2222</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T14" s="3">
         <v>0</v>
@@ -33824,7 +33824,7 @@
         <v>2221</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>2223</v>
@@ -33833,7 +33833,7 @@
         <v>2222</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T15" s="3">
         <v>0</v>
@@ -33886,7 +33886,7 @@
         <v>2221</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>2223</v>
@@ -33895,7 +33895,7 @@
         <v>2222</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T16" s="3">
         <v>0</v>
@@ -33948,7 +33948,7 @@
         <v>2221</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>2223</v>
@@ -33957,7 +33957,7 @@
         <v>2222</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T17" s="3">
         <v>0</v>
@@ -34010,7 +34010,7 @@
         <v>2221</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>2223</v>
@@ -34019,7 +34019,7 @@
         <v>2222</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T18" s="3">
         <v>0</v>
@@ -34072,7 +34072,7 @@
         <v>2221</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>2223</v>
@@ -34081,7 +34081,7 @@
         <v>2222</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T19" s="3">
         <v>0</v>
@@ -34234,7 +34234,7 @@
         <v>2221</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>2223</v>
@@ -34346,7 +34346,7 @@
         <v>2221</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>2223</v>
@@ -34758,7 +34758,7 @@
         <v>2221</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>2223</v>
@@ -34767,7 +34767,7 @@
         <v>2222</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T32" s="3">
         <v>0</v>
@@ -34820,7 +34820,7 @@
         <v>2221</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>2223</v>
@@ -34829,7 +34829,7 @@
         <v>2222</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T33" s="3">
         <v>0</v>
@@ -34882,7 +34882,7 @@
         <v>2221</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>2223</v>
@@ -34891,7 +34891,7 @@
         <v>2222</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T34" s="3">
         <v>0</v>
@@ -34944,7 +34944,7 @@
         <v>2221</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>2223</v>
@@ -34953,7 +34953,7 @@
         <v>2222</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T35" s="3">
         <v>0</v>
@@ -35006,7 +35006,7 @@
         <v>2221</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>2223</v>
@@ -35015,7 +35015,7 @@
         <v>2222</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T36" s="3">
         <v>0</v>
@@ -35118,7 +35118,7 @@
         <v>2221</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="Q38" s="3" t="s">
         <v>2223</v>
@@ -35127,7 +35127,7 @@
         <v>2222</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T38" s="3">
         <v>0</v>
@@ -35180,7 +35180,7 @@
         <v>2221</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>2223</v>
@@ -35189,7 +35189,7 @@
         <v>2222</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T39" s="3">
         <v>0</v>
@@ -35342,7 +35342,7 @@
         <v>2221</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>2223</v>
@@ -35351,7 +35351,7 @@
         <v>2222</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T42" s="3">
         <v>0</v>
@@ -35404,7 +35404,7 @@
         <v>2221</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>2223</v>
@@ -35413,7 +35413,7 @@
         <v>2222</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T43" s="3">
         <v>0</v>
@@ -35466,7 +35466,7 @@
         <v>2221</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>2223</v>
@@ -35475,7 +35475,7 @@
         <v>2222</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T44" s="3">
         <v>0</v>
@@ -35528,7 +35528,7 @@
         <v>2221</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>2223</v>
@@ -35537,7 +35537,7 @@
         <v>2222</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T45" s="3">
         <v>0</v>
@@ -35590,7 +35590,7 @@
         <v>2221</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>2223</v>
@@ -35599,7 +35599,7 @@
         <v>2222</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T46" s="3">
         <v>0</v>
@@ -35702,7 +35702,7 @@
         <v>2221</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>2223</v>
@@ -35711,7 +35711,7 @@
         <v>2222</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T48" s="3">
         <v>0</v>
@@ -35764,7 +35764,7 @@
         <v>2221</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="Q49" s="3" t="s">
         <v>2223</v>
@@ -35773,7 +35773,7 @@
         <v>2222</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T49" s="3">
         <v>0</v>
@@ -35926,7 +35926,7 @@
         <v>2221</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="Q52" s="3" t="s">
         <v>2223</v>
@@ -35935,7 +35935,7 @@
         <v>2222</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T52" s="3">
         <v>0</v>
@@ -35988,7 +35988,7 @@
         <v>2221</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>2223</v>
@@ -35997,7 +35997,7 @@
         <v>2222</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T53" s="3">
         <v>0</v>
@@ -36050,7 +36050,7 @@
         <v>2221</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>2223</v>
@@ -36059,7 +36059,7 @@
         <v>2222</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T54" s="3">
         <v>0</v>
@@ -36112,7 +36112,7 @@
         <v>2221</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>2223</v>
@@ -36121,7 +36121,7 @@
         <v>2222</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T55" s="3">
         <v>0</v>
@@ -36174,7 +36174,7 @@
         <v>2221</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>2223</v>
@@ -36183,7 +36183,7 @@
         <v>2222</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T56" s="3">
         <v>0</v>
@@ -36236,7 +36236,7 @@
         <v>2221</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>2223</v>
@@ -36245,7 +36245,7 @@
         <v>2222</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T57" s="3">
         <v>0</v>
@@ -36298,7 +36298,7 @@
         <v>2221</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="Q58" s="3" t="s">
         <v>2223</v>
@@ -36307,7 +36307,7 @@
         <v>2222</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T58" s="3">
         <v>0</v>
@@ -36360,7 +36360,7 @@
         <v>2221</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>2223</v>
@@ -36369,7 +36369,7 @@
         <v>2222</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="T59" s="3">
         <v>0</v>
@@ -36516,7 +36516,7 @@
         <v>2350</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="Q62" s="3">
         <v>0</v>
@@ -36525,7 +36525,7 @@
         <v>2650</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="T62" s="3">
         <v>0</v>
@@ -36574,7 +36574,7 @@
         <v>2346</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="Q63" s="3">
         <v>0</v>
@@ -36583,7 +36583,7 @@
         <v>2651</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="T63" s="3">
         <v>0</v>
@@ -36636,7 +36636,7 @@
         <v>539</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="Q64" s="3" t="s">
         <v>540</v>
@@ -36645,7 +36645,7 @@
         <v>541</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="T64" s="3">
         <v>0</v>
@@ -36760,7 +36760,7 @@
         <v>539</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="Q66" s="3" t="s">
         <v>540</v>
@@ -36769,7 +36769,7 @@
         <v>541</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="T66" s="3">
         <v>0</v>
@@ -37256,7 +37256,7 @@
         <v>539</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="Q74" s="3" t="s">
         <v>540</v>
@@ -37291,7 +37291,7 @@
         <v>93</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="H75" s="57">
         <v>518</v>
@@ -37318,7 +37318,7 @@
         <v>539</v>
       </c>
       <c r="P75" s="3" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="Q75" s="3" t="s">
         <v>540</v>
@@ -37380,7 +37380,7 @@
         <v>532</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="Q76" s="3" t="s">
         <v>533</v>
@@ -37389,7 +37389,7 @@
         <v>534</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="77" spans="1:20" s="73" customFormat="1" ht="30">
@@ -37901,7 +37901,7 @@
       <c r="N86" s="72"/>
       <c r="O86" s="72"/>
       <c r="P86" s="3" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="Q86" s="3" t="s">
         <v>533</v>
@@ -37910,7 +37910,7 @@
         <v>534</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="T86" s="3"/>
     </row>
@@ -37934,7 +37934,7 @@
         <v>93</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="H87" s="55">
         <v>515</v>
@@ -37961,7 +37961,7 @@
         <v>532</v>
       </c>
       <c r="P87" s="3" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="Q87" s="3" t="s">
         <v>533</v>
@@ -37970,7 +37970,7 @@
         <v>534</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="T87" s="3"/>
     </row>
@@ -38079,7 +38079,7 @@
         <v>122</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="Q89" s="3" t="s">
         <v>217</v>
@@ -38141,7 +38141,7 @@
         <v>122</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="Q90" s="3" t="s">
         <v>217</v>
@@ -38203,7 +38203,7 @@
         <v>122</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="Q91" s="3" t="s">
         <v>217</v>
@@ -38265,7 +38265,7 @@
         <v>122</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>217</v>
@@ -38513,7 +38513,7 @@
         <v>122</v>
       </c>
       <c r="P96" s="3" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="Q96" s="3" t="s">
         <v>217</v>
@@ -38637,7 +38637,7 @@
         <v>122</v>
       </c>
       <c r="P98" s="3" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="Q98" s="3" t="s">
         <v>217</v>
@@ -38699,7 +38699,7 @@
         <v>122</v>
       </c>
       <c r="P99" s="3" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="Q99" s="3" t="s">
         <v>217</v>
@@ -38734,7 +38734,7 @@
         <v>93</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="H100" s="55">
         <v>373</v>
@@ -38761,7 +38761,7 @@
         <v>122</v>
       </c>
       <c r="P100" s="3" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="Q100" s="3" t="s">
         <v>217</v>
@@ -38823,7 +38823,7 @@
         <v>539</v>
       </c>
       <c r="P101" s="3" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="Q101" s="3" t="s">
         <v>540</v>
@@ -38882,7 +38882,7 @@
         <v>539</v>
       </c>
       <c r="P102" s="3" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="Q102" s="3" t="s">
         <v>540</v>
@@ -38942,7 +38942,7 @@
         <v>539</v>
       </c>
       <c r="P103" s="3" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="Q103" s="3" t="s">
         <v>540</v>
@@ -39002,7 +39002,7 @@
         <v>539</v>
       </c>
       <c r="P104" s="3" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="Q104" s="3" t="s">
         <v>540</v>
@@ -39453,7 +39453,7 @@
         <v>93</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="H112" s="55">
         <v>511</v>
@@ -39480,7 +39480,7 @@
         <v>539</v>
       </c>
       <c r="P112" s="3" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="Q112" s="3" t="s">
         <v>540</v>
@@ -39536,7 +39536,7 @@
         <v>544</v>
       </c>
       <c r="P113" s="3" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="Q113" s="3" t="s">
         <v>545</v>
@@ -39681,7 +39681,7 @@
         <v>315</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>131</v>
@@ -39739,7 +39739,7 @@
         <v>315</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>132</v>
@@ -39789,7 +39789,7 @@
         <v>315</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>134</v>
@@ -39839,7 +39839,7 @@
         <v>315</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>135</v>
@@ -39869,7 +39869,7 @@
         <v>124</v>
       </c>
       <c r="P119" s="3" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
       <c r="Q119" s="3" t="s">
         <v>221</v>
@@ -39897,7 +39897,7 @@
         <v>315</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>136</v>
@@ -39927,7 +39927,7 @@
         <v>124</v>
       </c>
       <c r="P120" s="3" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="Q120" s="3" t="s">
         <v>221</v>
@@ -39955,7 +39955,7 @@
         <v>316</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>131</v>
@@ -39994,7 +39994,7 @@
         <v>316</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>132</v>
@@ -40040,7 +40040,7 @@
         <v>316</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>134</v>
@@ -40086,7 +40086,7 @@
         <v>316</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>135</v>
@@ -40116,7 +40116,7 @@
         <v>124</v>
       </c>
       <c r="P124" s="3" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
       <c r="Q124" s="3" t="s">
         <v>221</v>
@@ -40144,7 +40144,7 @@
         <v>316</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>136</v>
@@ -40174,7 +40174,7 @@
         <v>124</v>
       </c>
       <c r="P125" s="3" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="Q125" s="3" t="s">
         <v>221</v>
@@ -40363,7 +40363,7 @@
         <v>124</v>
       </c>
       <c r="P129" s="3" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
       <c r="Q129" s="3" t="s">
         <v>221</v>
@@ -40449,7 +40449,7 @@
         <v>315</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>131</v>
@@ -40511,7 +40511,7 @@
         <v>315</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>132</v>
@@ -40541,7 +40541,7 @@
         <v>36</v>
       </c>
       <c r="P132" s="3" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="Q132" s="3" t="s">
         <v>223</v>
@@ -40571,7 +40571,7 @@
         <v>315</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>133</v>
@@ -40601,7 +40601,7 @@
         <v>36</v>
       </c>
       <c r="P133" s="3" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="Q133" s="3" t="s">
         <v>223</v>
@@ -40631,7 +40631,7 @@
         <v>315</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>134</v>
@@ -40661,7 +40661,7 @@
         <v>36</v>
       </c>
       <c r="P134" s="3" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="Q134" s="3" t="s">
         <v>223</v>
@@ -40691,7 +40691,7 @@
         <v>315</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>135</v>
@@ -40721,7 +40721,7 @@
         <v>36</v>
       </c>
       <c r="P135" s="3" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
       <c r="Q135" s="3" t="s">
         <v>223</v>
@@ -40753,7 +40753,7 @@
         <v>315</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>136</v>
@@ -40783,7 +40783,7 @@
         <v>36</v>
       </c>
       <c r="P136" s="3" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="Q136" s="3" t="s">
         <v>223</v>
@@ -40815,7 +40815,7 @@
         <v>316</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>131</v>
@@ -40877,7 +40877,7 @@
         <v>316</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G138" s="3" t="s">
         <v>132</v>
@@ -40907,7 +40907,7 @@
         <v>36</v>
       </c>
       <c r="P138" s="3" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="Q138" s="3" t="s">
         <v>223</v>
@@ -40939,7 +40939,7 @@
         <v>316</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G139" s="3" t="s">
         <v>133</v>
@@ -40969,7 +40969,7 @@
         <v>36</v>
       </c>
       <c r="P139" s="3" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="Q139" s="3" t="s">
         <v>223</v>
@@ -41001,7 +41001,7 @@
         <v>316</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G140" s="3" t="s">
         <v>134</v>
@@ -41031,7 +41031,7 @@
         <v>36</v>
       </c>
       <c r="P140" s="3" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="Q140" s="3" t="s">
         <v>223</v>
@@ -41063,7 +41063,7 @@
         <v>316</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>135</v>
@@ -41093,7 +41093,7 @@
         <v>36</v>
       </c>
       <c r="P141" s="3" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="Q141" s="3" t="s">
         <v>223</v>
@@ -41125,7 +41125,7 @@
         <v>316</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G142" s="3" t="s">
         <v>136</v>
@@ -41155,7 +41155,7 @@
         <v>36</v>
       </c>
       <c r="P142" s="3" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="Q142" s="3" t="s">
         <v>223</v>
@@ -41279,7 +41279,7 @@
         <v>36</v>
       </c>
       <c r="P144" s="3" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="Q144" s="3" t="s">
         <v>223</v>
@@ -41341,7 +41341,7 @@
         <v>36</v>
       </c>
       <c r="P145" s="3" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="Q145" s="3" t="s">
         <v>223</v>
@@ -41403,7 +41403,7 @@
         <v>36</v>
       </c>
       <c r="P146" s="3" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="Q146" s="3" t="s">
         <v>223</v>
@@ -41465,7 +41465,7 @@
         <v>36</v>
       </c>
       <c r="P147" s="3" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="Q147" s="3" t="s">
         <v>223</v>
@@ -41527,7 +41527,7 @@
         <v>36</v>
       </c>
       <c r="P148" s="3" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="Q148" s="3" t="s">
         <v>223</v>
@@ -41641,7 +41641,7 @@
         <v>298</v>
       </c>
       <c r="P150" s="3" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="Q150" s="3" t="s">
         <v>299</v>
@@ -41699,7 +41699,7 @@
         <v>305</v>
       </c>
       <c r="P151" s="3" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="Q151" s="3" t="s">
         <v>302</v>
@@ -41783,7 +41783,7 @@
       </c>
       <c r="E153" s="54"/>
       <c r="F153" s="3" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>213</v>
@@ -41813,7 +41813,7 @@
         <v>2358</v>
       </c>
       <c r="P153" s="3" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="Q153" s="3" t="s">
         <v>229</v>
@@ -41841,7 +41841,7 @@
       </c>
       <c r="E154" s="54"/>
       <c r="F154" s="3" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>213</v>
@@ -41871,7 +41871,7 @@
         <v>2358</v>
       </c>
       <c r="P154" s="3" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="Q154" s="3" t="s">
         <v>229</v>
@@ -41929,7 +41929,7 @@
         <v>2358</v>
       </c>
       <c r="P155" s="3" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="Q155" s="3" t="s">
         <v>229</v>
@@ -42153,7 +42153,7 @@
         <v>34</v>
       </c>
       <c r="P159" s="3" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="Q159" s="3" t="s">
         <v>231</v>
@@ -42269,7 +42269,7 @@
         <v>34</v>
       </c>
       <c r="P161" s="3" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="Q161" s="3" t="s">
         <v>231</v>
@@ -43083,7 +43083,7 @@
         <v>40</v>
       </c>
       <c r="P177" s="3" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="Q177" s="3" t="s">
         <v>2325</v>
@@ -43139,7 +43139,7 @@
         <v>310</v>
       </c>
       <c r="P178" s="3" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="Q178" s="3" t="s">
         <v>312</v>
@@ -43148,7 +43148,7 @@
         <v>314</v>
       </c>
       <c r="S178" s="3" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="179" spans="1:20" s="3" customFormat="1" ht="45">
@@ -43194,7 +43194,7 @@
         <v>311</v>
       </c>
       <c r="P179" s="3" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="Q179" s="3" t="s">
         <v>313</v>
@@ -43203,7 +43203,7 @@
         <v>314</v>
       </c>
       <c r="S179" s="3" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="180" spans="1:20" ht="45">
@@ -43297,7 +43297,7 @@
         <v>39</v>
       </c>
       <c r="P181" s="3" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="Q181" s="3" t="s">
         <v>233</v>
@@ -43355,7 +43355,7 @@
         <v>212</v>
       </c>
       <c r="P182" s="3" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="Q182" s="3" t="s">
         <v>235</v>
@@ -43364,10 +43364,10 @@
         <v>236</v>
       </c>
       <c r="S182" s="3" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="T182" s="3" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="183" spans="1:20" ht="45">
@@ -44183,7 +44183,7 @@
         <v>35</v>
       </c>
       <c r="P198" s="3" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="Q198" s="3" t="s">
         <v>237</v>
@@ -44241,7 +44241,7 @@
         <v>144</v>
       </c>
       <c r="P199" s="3" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="Q199" s="3" t="s">
         <v>239</v>
@@ -47735,7 +47735,7 @@
         <v>286</v>
       </c>
       <c r="P266" s="3" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="Q266" s="3" t="s">
         <v>1951</v>
@@ -47744,7 +47744,7 @@
         <v>287</v>
       </c>
       <c r="S266" s="3" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="T266" s="3">
         <v>0</v>
@@ -48623,7 +48623,7 @@
         <v>39</v>
       </c>
       <c r="P282" s="3" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="Q282" s="3" t="s">
         <v>248</v>
@@ -48743,7 +48743,7 @@
         <v>36</v>
       </c>
       <c r="P284" s="3" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="Q284" s="3" t="s">
         <v>250</v>
@@ -49103,7 +49103,7 @@
         <v>36</v>
       </c>
       <c r="P290" s="3" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="Q290" s="3" t="s">
         <v>250</v>
@@ -49161,7 +49161,7 @@
         <v>39</v>
       </c>
       <c r="P291" s="3" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="Q291" s="3" t="s">
         <v>252</v>
@@ -53625,7 +53625,7 @@
         <v>2255</v>
       </c>
       <c r="P363" s="3" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="Q363" s="3" t="s">
         <v>254</v>
@@ -53687,7 +53687,7 @@
         <v>2255</v>
       </c>
       <c r="P364" s="3" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="Q364" s="3" t="s">
         <v>254</v>
@@ -53997,7 +53997,7 @@
         <v>2255</v>
       </c>
       <c r="P369" s="3" t="s">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="Q369" s="3" t="s">
         <v>254</v>
@@ -54059,7 +54059,7 @@
         <v>2255</v>
       </c>
       <c r="P370" s="3" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="Q370" s="3" t="s">
         <v>254</v>
@@ -54421,7 +54421,7 @@
         <v>2305</v>
       </c>
       <c r="P376" s="3" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="Q376" s="3">
         <v>0</v>
@@ -55181,7 +55181,7 @@
         <v>39</v>
       </c>
       <c r="P389" s="3" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="Q389" s="3" t="s">
         <v>259</v>
@@ -55909,7 +55909,7 @@
         <v>2383</v>
       </c>
       <c r="P402" s="3" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="Q402" s="3">
         <v>0</v>
@@ -55967,7 +55967,7 @@
         <v>39</v>
       </c>
       <c r="P403" s="3" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="Q403" s="3" t="s">
         <v>273</v>
@@ -56027,7 +56027,7 @@
         <v>161</v>
       </c>
       <c r="P404" s="3" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="Q404" s="3" t="s">
         <v>275</v>
@@ -56036,10 +56036,10 @@
         <v>276</v>
       </c>
       <c r="S404" s="3" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="T404" s="3" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="405" spans="1:20" s="6" customFormat="1" ht="75">
@@ -56087,7 +56087,7 @@
         <v>161</v>
       </c>
       <c r="P405" s="3" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="Q405" s="3" t="s">
         <v>275</v>
@@ -56147,7 +56147,7 @@
         <v>161</v>
       </c>
       <c r="P406" s="3" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="Q406" s="3" t="s">
         <v>275</v>
@@ -56207,7 +56207,7 @@
         <v>161</v>
       </c>
       <c r="P407" s="3" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
       <c r="Q407" s="3" t="s">
         <v>275</v>
@@ -56267,7 +56267,7 @@
         <v>161</v>
       </c>
       <c r="P408" s="3" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="Q408" s="3" t="s">
         <v>275</v>
@@ -58565,7 +58565,7 @@
         <v>165</v>
       </c>
       <c r="P452" s="3" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
       <c r="Q452" s="3" t="s">
         <v>281</v>
@@ -58574,7 +58574,7 @@
         <v>282</v>
       </c>
       <c r="S452" s="3" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="T452" s="3">
         <v>0</v>
@@ -58625,7 +58625,7 @@
         <v>165</v>
       </c>
       <c r="P453" s="3" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
       <c r="Q453" s="3" t="s">
         <v>281</v>
@@ -58634,7 +58634,7 @@
         <v>282</v>
       </c>
       <c r="S453" s="3" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="T453" s="3">
         <v>0</v>
@@ -58685,7 +58685,7 @@
         <v>165</v>
       </c>
       <c r="P454" s="3" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="Q454" s="3" t="s">
         <v>281</v>
@@ -58694,7 +58694,7 @@
         <v>282</v>
       </c>
       <c r="S454" s="3" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="T454" s="3">
         <v>0</v>
@@ -58849,7 +58849,7 @@
         <v>165</v>
       </c>
       <c r="P457" s="3" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="Q457" s="3" t="s">
         <v>281</v>
@@ -58858,7 +58858,7 @@
         <v>282</v>
       </c>
       <c r="S457" s="3" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="T457" s="3">
         <v>0</v>
@@ -58909,7 +58909,7 @@
         <v>165</v>
       </c>
       <c r="P458" s="3" t="s">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="Q458" s="3" t="s">
         <v>281</v>
@@ -58918,7 +58918,7 @@
         <v>282</v>
       </c>
       <c r="S458" s="3" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="T458" s="3">
         <v>0</v>
@@ -61303,7 +61303,7 @@
       </c>
       <c r="E500" s="54"/>
       <c r="F500" s="3" t="s">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="G500" s="3" t="s">
         <v>213</v>
@@ -61333,7 +61333,7 @@
         <v>37</v>
       </c>
       <c r="P500" s="3" t="s">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="Q500" s="3" t="s">
         <v>283</v>
@@ -61363,7 +61363,7 @@
       </c>
       <c r="E501" s="54"/>
       <c r="F501" s="3" t="s">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="G501" s="3"/>
       <c r="H501" s="55">
@@ -61391,7 +61391,7 @@
         <v>37</v>
       </c>
       <c r="P501" s="3" t="s">
-        <v>3007</v>
+        <v>3006</v>
       </c>
       <c r="Q501" s="3" t="s">
         <v>283</v>
@@ -63223,7 +63223,7 @@
       </c>
       <c r="E533" s="54"/>
       <c r="F533" s="3" t="s">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="G533" s="3" t="s">
         <v>213</v>
@@ -63253,7 +63253,7 @@
         <v>38</v>
       </c>
       <c r="P533" s="3" t="s">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="Q533" s="3" t="s">
         <v>283</v>
@@ -63282,7 +63282,7 @@
         <v>2438</v>
       </c>
       <c r="F534" s="5" t="s">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="H534" s="238">
         <v>519</v>
@@ -63309,7 +63309,7 @@
         <v>38</v>
       </c>
       <c r="P534" s="3" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="Q534" s="3" t="s">
         <v>283</v>
@@ -63767,7 +63767,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -64367,13 +64367,13 @@
         <v>416</v>
       </c>
       <c r="F27" s="156" t="s">
+        <v>2920</v>
+      </c>
+      <c r="G27" s="162" t="s">
         <v>2921</v>
       </c>
-      <c r="G27" s="162" t="s">
+      <c r="H27" s="156" t="s">
         <v>2922</v>
-      </c>
-      <c r="H27" s="156" t="s">
-        <v>2923</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="60">
@@ -64393,13 +64393,13 @@
         <v>416</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>2923</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>2924</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>2925</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>2926</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="60.75" thickBot="1">
@@ -64590,7 +64590,7 @@
         <v>508</v>
       </c>
       <c r="E37" s="162" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="F37" s="162" t="s">
         <v>2272</v>
@@ -64611,7 +64611,7 @@
         <v>508</v>
       </c>
       <c r="E38" s="162" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="F38" s="162" t="s">
         <v>2272</v>
@@ -64632,7 +64632,7 @@
         <v>508</v>
       </c>
       <c r="E39" s="162" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="F39" s="162" t="s">
         <v>2268</v>
@@ -64653,7 +64653,7 @@
         <v>508</v>
       </c>
       <c r="E40" s="224" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="F40" s="224" t="s">
         <v>2268</v>
@@ -64675,7 +64675,7 @@
         <v>72</v>
       </c>
       <c r="E41" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F41" s="162" t="s">
         <v>2275</v>
@@ -64701,7 +64701,7 @@
         <v>72</v>
       </c>
       <c r="E42" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F42" s="162" t="s">
         <v>2735</v>
@@ -64722,7 +64722,7 @@
         <v>72</v>
       </c>
       <c r="E43" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F43" s="162" t="s">
         <v>2276</v>
@@ -64748,7 +64748,7 @@
         <v>72</v>
       </c>
       <c r="E44" s="224" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F44" s="224" t="s">
         <v>2736</v>
@@ -64770,7 +64770,7 @@
         <v>72</v>
       </c>
       <c r="E45" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>2600</v>
@@ -64796,7 +64796,7 @@
         <v>72</v>
       </c>
       <c r="E46" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>2613</v>
@@ -64822,7 +64822,7 @@
         <v>72</v>
       </c>
       <c r="E47" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>2624</v>
@@ -64848,7 +64848,7 @@
         <v>72</v>
       </c>
       <c r="E48" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>2618</v>
@@ -64874,7 +64874,7 @@
         <v>72</v>
       </c>
       <c r="E49" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>2619</v>
@@ -64900,7 +64900,7 @@
         <v>72</v>
       </c>
       <c r="E50" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>2625</v>
@@ -64926,7 +64926,7 @@
         <v>72</v>
       </c>
       <c r="E51" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>2626</v>
@@ -64952,7 +64952,7 @@
         <v>72</v>
       </c>
       <c r="E52" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>2627</v>
@@ -64978,7 +64978,7 @@
         <v>72</v>
       </c>
       <c r="E53" s="162" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>2646</v>
@@ -65004,7 +65004,7 @@
         <v>72</v>
       </c>
       <c r="E54" s="224" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F54" s="235" t="s">
         <v>2647</v>
@@ -65051,7 +65051,7 @@
         <v>72</v>
       </c>
       <c r="E56" s="196" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F56" s="196" t="s">
         <v>75</v>
@@ -65203,7 +65203,7 @@
         <v>2190</v>
       </c>
       <c r="E62" s="156" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="F62" s="156" t="s">
         <v>2419</v>
@@ -65310,13 +65310,13 @@
         <v>2216</v>
       </c>
       <c r="F66" s="157" t="s">
+        <v>2945</v>
+      </c>
+      <c r="G66" s="225" t="s">
+        <v>2944</v>
+      </c>
+      <c r="H66" s="157" t="s">
         <v>2946</v>
-      </c>
-      <c r="G66" s="225" t="s">
-        <v>2945</v>
-      </c>
-      <c r="H66" s="157" t="s">
-        <v>2947</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="30.75" thickBot="1">
@@ -65336,13 +65336,13 @@
         <v>2217</v>
       </c>
       <c r="F67" s="196" t="s">
+        <v>2926</v>
+      </c>
+      <c r="G67" s="224" t="s">
         <v>2927</v>
       </c>
-      <c r="G67" s="224" t="s">
+      <c r="H67" s="196" t="s">
         <v>2928</v>
-      </c>
-      <c r="H67" s="196" t="s">
-        <v>2929</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="90">
@@ -65480,7 +65480,7 @@
         <v>2738</v>
       </c>
       <c r="B73" s="157" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="C73" s="156" t="s">
         <v>73</v>
@@ -65492,7 +65492,7 @@
         <v>2195</v>
       </c>
       <c r="F73" s="156" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="G73" s="156" t="s">
         <v>2541</v>
@@ -65636,7 +65636,7 @@
         <v>2738</v>
       </c>
       <c r="B79" s="195" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="C79" s="196" t="s">
         <v>73</v>
@@ -65648,7 +65648,7 @@
         <v>2194</v>
       </c>
       <c r="F79" s="196" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="G79" s="196" t="s">
         <v>2541</v>
@@ -65674,13 +65674,13 @@
         <v>416</v>
       </c>
       <c r="F80" s="157" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="G80" s="157" t="s">
+        <v>2947</v>
+      </c>
+      <c r="H80" s="157" t="s">
         <v>2948</v>
-      </c>
-      <c r="H80" s="157" t="s">
-        <v>2949</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="90">
@@ -65700,13 +65700,13 @@
         <v>529</v>
       </c>
       <c r="F81" s="157" t="s">
+        <v>2929</v>
+      </c>
+      <c r="G81" s="157" t="s">
         <v>2930</v>
       </c>
-      <c r="G81" s="157" t="s">
+      <c r="H81" s="157" t="s">
         <v>2931</v>
-      </c>
-      <c r="H81" s="157" t="s">
-        <v>2932</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="75.75" thickBot="1">
@@ -65726,13 +65726,13 @@
         <v>529</v>
       </c>
       <c r="F82" s="195" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="G82" s="195" t="s">
+        <v>2947</v>
+      </c>
+      <c r="H82" s="195" t="s">
         <v>2948</v>
-      </c>
-      <c r="H82" s="195" t="s">
-        <v>2949</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="60">
@@ -65960,13 +65960,13 @@
         <v>529</v>
       </c>
       <c r="F91" s="157" t="s">
+        <v>2955</v>
+      </c>
+      <c r="G91" s="225" t="s">
         <v>2956</v>
       </c>
-      <c r="G91" s="225" t="s">
+      <c r="H91" s="156" t="s">
         <v>2957</v>
-      </c>
-      <c r="H91" s="156" t="s">
-        <v>2958</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="30">
@@ -65989,7 +65989,7 @@
         <v>2213</v>
       </c>
       <c r="G92" s="225" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="H92" s="156" t="s">
         <v>2196</v>
@@ -66012,13 +66012,13 @@
         <v>529</v>
       </c>
       <c r="F93" s="195" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="G93" s="195" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="H93" s="196" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="75">
@@ -66038,13 +66038,13 @@
         <v>529</v>
       </c>
       <c r="F94" s="157" t="s">
+        <v>2961</v>
+      </c>
+      <c r="G94" s="157" t="s">
         <v>2962</v>
       </c>
-      <c r="G94" s="157" t="s">
+      <c r="H94" s="157" t="s">
         <v>2963</v>
-      </c>
-      <c r="H94" s="157" t="s">
-        <v>2964</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="45">
@@ -66064,13 +66064,13 @@
         <v>529</v>
       </c>
       <c r="F95" s="157" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="G95" s="157" t="s">
+        <v>2921</v>
+      </c>
+      <c r="H95" s="157" t="s">
         <v>2922</v>
-      </c>
-      <c r="H95" s="157" t="s">
-        <v>2923</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -66350,7 +66350,7 @@
         <v>74</v>
       </c>
       <c r="E108" s="157" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F108" s="156" t="s">
         <v>2581</v>
@@ -66376,7 +66376,7 @@
         <v>72</v>
       </c>
       <c r="E109" s="157" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F109" s="156" t="s">
         <v>2582</v>
@@ -66454,7 +66454,7 @@
         <v>74</v>
       </c>
       <c r="E112" s="157" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F112" s="156" t="s">
         <v>2716</v>
@@ -66480,7 +66480,7 @@
         <v>72</v>
       </c>
       <c r="E113" s="157" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="F113" s="156" t="s">
         <v>2717</v>
@@ -66558,7 +66558,7 @@
         <v>2190</v>
       </c>
       <c r="E116" s="157" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="F116" s="156" t="s">
         <v>2583</v>
@@ -66584,7 +66584,7 @@
         <v>2190</v>
       </c>
       <c r="E117" s="157" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="F117" s="156" t="s">
         <v>2594</v>
@@ -66610,7 +66610,7 @@
         <v>2190</v>
       </c>
       <c r="E118" s="157" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="F118" s="156" t="s">
         <v>2204</v>
@@ -66636,7 +66636,7 @@
         <v>2190</v>
       </c>
       <c r="E119" s="157" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="F119" s="156" t="s">
         <v>2586</v>
@@ -66662,7 +66662,7 @@
         <v>2190</v>
       </c>
       <c r="E120" s="157" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="F120" s="156" t="s">
         <v>2206</v>
@@ -66688,7 +66688,7 @@
         <v>2190</v>
       </c>
       <c r="E121" s="157" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="F121" s="156" t="s">
         <v>2589</v>
@@ -66714,7 +66714,7 @@
         <v>2190</v>
       </c>
       <c r="E122" s="157" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="F122" s="156" t="s">
         <v>2590</v>
@@ -66740,7 +66740,7 @@
         <v>2190</v>
       </c>
       <c r="E123" s="157" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="F123" s="156" t="s">
         <v>2706</v>
@@ -66766,7 +66766,7 @@
         <v>2190</v>
       </c>
       <c r="E124" s="157" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="F124" s="156" t="s">
         <v>2597</v>
@@ -66792,7 +66792,7 @@
         <v>2190</v>
       </c>
       <c r="E125" s="195" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="F125" s="196" t="s">
         <v>2772</v>
@@ -66818,7 +66818,7 @@
         <v>72</v>
       </c>
       <c r="E126" s="157" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="F126" s="156" t="s">
         <v>2207</v>
@@ -66839,7 +66839,7 @@
         <v>72</v>
       </c>
       <c r="E127" s="157" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="F127" s="156" t="s">
         <v>2211</v>
@@ -66865,7 +66865,7 @@
         <v>72</v>
       </c>
       <c r="E128" s="157" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="F128" s="156" t="s">
         <v>2208</v>
@@ -66886,7 +66886,7 @@
         <v>72</v>
       </c>
       <c r="E129" s="157" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="F129" s="156" t="s">
         <v>2209</v>
@@ -66907,7 +66907,7 @@
         <v>72</v>
       </c>
       <c r="E130" s="156" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="F130" s="156" t="s">
         <v>2210</v>
@@ -66928,7 +66928,7 @@
         <v>72</v>
       </c>
       <c r="E131" s="196" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="F131" s="196" t="s">
         <v>2389</v>
@@ -68051,7 +68051,7 @@
       </c>
       <c r="C99" s="167"/>
       <c r="D99" s="165" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -69109,7 +69109,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="229" t="s">
-        <v>2777</v>
+        <v>3007</v>
       </c>
       <c r="B2" s="229" t="s">
         <v>82</v>
@@ -69117,10 +69117,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="229" t="s">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="B3" s="229" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -69187,7 +69187,7 @@
     </row>
     <row r="2" spans="1:26" ht="60">
       <c r="A2" s="199" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="B2" s="199">
         <v>2030</v>
@@ -69201,7 +69201,7 @@
         <v>30.488000000000003</v>
       </c>
       <c r="E2" s="199" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="K2"/>
       <c r="L2"/>
@@ -69242,7 +69242,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="5" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="K4"/>
       <c r="L4"/>
@@ -69263,7 +69263,7 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="200" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="K5"/>
       <c r="L5"/>
@@ -69320,11 +69320,11 @@
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1">
       <c r="A8" s="201" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="B8" s="255"/>
       <c r="C8" s="257" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="D8" s="257"/>
       <c r="E8" s="257"/>
@@ -69350,11 +69350,11 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A9" s="206" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="B9" s="256"/>
       <c r="C9" s="260" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="D9" s="260"/>
       <c r="E9" s="260"/>
@@ -69381,21 +69381,21 @@
     <row r="10" spans="1:26" ht="49.5" customHeight="1">
       <c r="A10" s="207"/>
       <c r="B10" s="261" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="C10" s="257"/>
       <c r="D10" s="262"/>
       <c r="E10" s="203" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="F10" s="203" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G10" s="203" t="s">
+        <v>2860</v>
+      </c>
+      <c r="H10" s="203" t="s">
         <v>2838</v>
-      </c>
-      <c r="G10" s="203" t="s">
-        <v>2861</v>
-      </c>
-      <c r="H10" s="203" t="s">
-        <v>2839</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -69417,21 +69417,21 @@
     <row r="11" spans="1:26" ht="105" customHeight="1">
       <c r="A11" s="207"/>
       <c r="B11" s="265" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="C11" s="266"/>
       <c r="D11" s="267"/>
       <c r="E11" s="263" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="F11" s="263" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="G11" s="263" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="H11" s="263" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
@@ -69453,13 +69453,13 @@
     <row r="12" spans="1:26" ht="33">
       <c r="A12" s="207"/>
       <c r="B12" s="203" t="s">
+        <v>2840</v>
+      </c>
+      <c r="C12" s="203" t="s">
         <v>2841</v>
       </c>
-      <c r="C12" s="203" t="s">
-        <v>2842</v>
-      </c>
       <c r="D12" s="202" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="E12" s="263"/>
       <c r="F12" s="263"/>
@@ -69485,13 +69485,13 @@
     <row r="13" spans="1:26" ht="45">
       <c r="A13" s="217"/>
       <c r="B13" s="218" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="C13" s="219" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="D13" s="220" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="E13" s="264"/>
       <c r="F13" s="264"/>
@@ -70650,7 +70650,7 @@
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="253" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="B41" s="211">
         <v>26600</v>
@@ -70732,7 +70732,7 @@
     </row>
     <row r="43" spans="1:26">
       <c r="A43" s="204" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="B43" s="155"/>
       <c r="C43" s="155"/>
@@ -70760,7 +70760,7 @@
     </row>
     <row r="44" spans="1:26">
       <c r="A44" s="215" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="B44" s="155"/>
       <c r="C44" s="155"/>
@@ -70788,7 +70788,7 @@
     </row>
     <row r="45" spans="1:26">
       <c r="A45" s="205" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="B45" s="155"/>
       <c r="C45" s="155"/>
@@ -70816,7 +70816,7 @@
     </row>
     <row r="46" spans="1:26">
       <c r="A46" s="216" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="B46" s="155"/>
       <c r="C46" s="155"/>
@@ -70844,7 +70844,7 @@
     </row>
     <row r="47" spans="1:26">
       <c r="A47" s="215" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="B47" s="155"/>
       <c r="C47" s="155"/>
@@ -70872,7 +70872,7 @@
     </row>
     <row r="48" spans="1:26">
       <c r="A48" s="205" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="B48" s="155"/>
       <c r="C48" s="155"/>
@@ -70900,7 +70900,7 @@
     </row>
     <row r="49" spans="1:26">
       <c r="A49" s="216" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="B49" s="155"/>
       <c r="C49" s="155"/>
@@ -70928,7 +70928,7 @@
     </row>
     <row r="50" spans="1:26">
       <c r="A50" s="215" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="B50" s="155"/>
       <c r="C50" s="155"/>
@@ -70956,7 +70956,7 @@
     </row>
     <row r="51" spans="1:26">
       <c r="A51" s="205" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="B51" s="155"/>
       <c r="C51" s="155"/>
@@ -70984,7 +70984,7 @@
     </row>
     <row r="52" spans="1:26">
       <c r="A52" s="216" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="B52" s="155"/>
       <c r="C52" s="155"/>
@@ -71012,7 +71012,7 @@
     </row>
     <row r="53" spans="1:26">
       <c r="A53" s="215" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="B53" s="155"/>
       <c r="C53" s="155"/>
@@ -71040,7 +71040,7 @@
     </row>
     <row r="54" spans="1:26">
       <c r="A54" s="205" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="B54" s="155"/>
       <c r="C54" s="155"/>
@@ -71068,7 +71068,7 @@
     </row>
     <row r="55" spans="1:26">
       <c r="A55" s="216" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="B55" s="155"/>
       <c r="C55" s="155"/>
@@ -71096,7 +71096,7 @@
     </row>
     <row r="56" spans="1:26">
       <c r="A56" s="204" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="B56" s="155"/>
       <c r="C56" s="155"/>
@@ -71124,7 +71124,7 @@
     </row>
     <row r="57" spans="1:26">
       <c r="A57" s="215" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="B57" s="155"/>
       <c r="C57" s="155"/>
@@ -71152,7 +71152,7 @@
     </row>
     <row r="58" spans="1:26">
       <c r="A58" s="204" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="B58" s="155"/>
       <c r="C58" s="155"/>
@@ -81774,13 +81774,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
+      <c r="B1" s="268"/>
+      <c r="C1" s="268"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="272" t="s">
@@ -81849,13 +81849,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="271" t="s">
+      <c r="A60" s="268" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="271"/>
-      <c r="C60" s="271"/>
-      <c r="D60" s="271"/>
-      <c r="E60" s="271"/>
+      <c r="B60" s="268"/>
+      <c r="C60" s="268"/>
+      <c r="D60" s="268"/>
+      <c r="E60" s="268"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1">
       <c r="A85" s="11" t="s">
@@ -81960,13 +81960,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="271" t="s">
+      <c r="A89" s="268" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="271"/>
-      <c r="C89" s="271"/>
-      <c r="D89" s="271"/>
-      <c r="E89" s="271"/>
+      <c r="B89" s="268"/>
+      <c r="C89" s="268"/>
+      <c r="D89" s="268"/>
+      <c r="E89" s="268"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="11">
@@ -82053,13 +82053,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="271" t="s">
+      <c r="A98" s="268" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="271"/>
-      <c r="C98" s="271"/>
-      <c r="D98" s="271"/>
-      <c r="E98" s="271"/>
+      <c r="B98" s="268"/>
+      <c r="C98" s="268"/>
+      <c r="D98" s="268"/>
+      <c r="E98" s="268"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="19">
@@ -82143,13 +82143,13 @@
       <c r="A108" s="22"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="271" t="s">
+      <c r="A109" s="268" t="s">
         <v>187</v>
       </c>
-      <c r="B109" s="271"/>
-      <c r="C109" s="271"/>
-      <c r="D109" s="271"/>
-      <c r="E109" s="271"/>
+      <c r="B109" s="268"/>
+      <c r="C109" s="268"/>
+      <c r="D109" s="268"/>
+      <c r="E109" s="268"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1">
@@ -82162,13 +82162,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="271" t="s">
+      <c r="A113" s="268" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="271"/>
-      <c r="C113" s="271"/>
-      <c r="D113" s="271"/>
-      <c r="E113" s="271"/>
+      <c r="B113" s="268"/>
+      <c r="C113" s="268"/>
+      <c r="D113" s="268"/>
+      <c r="E113" s="268"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="19">
@@ -82249,13 +82249,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="271" t="s">
+      <c r="A124" s="268" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="271"/>
-      <c r="C124" s="271"/>
-      <c r="D124" s="271"/>
-      <c r="E124" s="271"/>
+      <c r="B124" s="268"/>
+      <c r="C124" s="268"/>
+      <c r="D124" s="268"/>
+      <c r="E124" s="268"/>
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:14">
@@ -82346,13 +82346,13 @@
       <c r="C133" s="17"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="271" t="s">
+      <c r="A134" s="268" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="271"/>
-      <c r="C134" s="271"/>
-      <c r="D134" s="271"/>
-      <c r="E134" s="271"/>
+      <c r="B134" s="268"/>
+      <c r="C134" s="268"/>
+      <c r="D134" s="268"/>
+      <c r="E134" s="268"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="29" t="s">
@@ -82367,25 +82367,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75">
       <c r="A136" s="31"/>
-      <c r="B136" s="268" t="s">
+      <c r="B136" s="269" t="s">
         <v>469</v>
       </c>
-      <c r="C136" s="269"/>
-      <c r="D136" s="269"/>
-      <c r="E136" s="270"/>
+      <c r="C136" s="270"/>
+      <c r="D136" s="270"/>
+      <c r="E136" s="271"/>
       <c r="F136" s="30"/>
       <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:14" ht="15.75">
       <c r="A137" s="32"/>
-      <c r="B137" s="268" t="s">
+      <c r="B137" s="269" t="s">
         <v>470</v>
       </c>
-      <c r="C137" s="270"/>
-      <c r="D137" s="268" t="s">
+      <c r="C137" s="271"/>
+      <c r="D137" s="269" t="s">
         <v>471</v>
       </c>
-      <c r="E137" s="270"/>
+      <c r="E137" s="271"/>
       <c r="F137" s="30"/>
       <c r="G137" s="30"/>
     </row>
@@ -82932,13 +82932,13 @@
       <c r="G163" s="30"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="271" t="s">
+      <c r="A165" s="268" t="s">
         <v>190</v>
       </c>
-      <c r="B165" s="271"/>
-      <c r="C165" s="271"/>
-      <c r="D165" s="271"/>
-      <c r="E165" s="271"/>
+      <c r="B165" s="268"/>
+      <c r="C165" s="268"/>
+      <c r="D165" s="268"/>
+      <c r="E165" s="268"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1">
       <c r="A166" s="25" t="s">
@@ -82961,10 +82961,10 @@
       <c r="B168" s="48"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="271" t="s">
+      <c r="A169" s="268" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="271"/>
+      <c r="B169" s="268"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="25" t="s">
@@ -82996,13 +82996,13 @@
       <c r="B173" s="48"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="271" t="s">
+      <c r="A174" s="268" t="s">
         <v>199</v>
       </c>
-      <c r="B174" s="271"/>
-      <c r="C174" s="271"/>
-      <c r="D174" s="271"/>
-      <c r="E174" s="271"/>
+      <c r="B174" s="268"/>
+      <c r="C174" s="268"/>
+      <c r="D174" s="268"/>
+      <c r="E174" s="268"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1">
       <c r="A175" s="25" t="s">
@@ -83022,13 +83022,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="271" t="s">
+      <c r="A178" s="268" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="271"/>
-      <c r="C178" s="271"/>
-      <c r="D178" s="271"/>
-      <c r="E178" s="271"/>
+      <c r="B178" s="268"/>
+      <c r="C178" s="268"/>
+      <c r="D178" s="268"/>
+      <c r="E178" s="268"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="27" t="s">
@@ -83056,13 +83056,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="271" t="s">
+      <c r="A183" s="268" t="s">
         <v>195</v>
       </c>
-      <c r="B183" s="271"/>
-      <c r="C183" s="271"/>
-      <c r="D183" s="271"/>
-      <c r="E183" s="271"/>
+      <c r="B183" s="268"/>
+      <c r="C183" s="268"/>
+      <c r="D183" s="268"/>
+      <c r="E183" s="268"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="25" t="s">
@@ -83117,13 +83117,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="271" t="s">
+      <c r="A191" s="268" t="s">
         <v>209</v>
       </c>
-      <c r="B191" s="271"/>
-      <c r="C191" s="271"/>
-      <c r="D191" s="271"/>
-      <c r="E191" s="271"/>
+      <c r="B191" s="268"/>
+      <c r="C191" s="268"/>
+      <c r="D191" s="268"/>
+      <c r="E191" s="268"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="23" t="s">
@@ -83183,12 +83183,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -83203,6 +83197,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -83211,21 +83211,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -83463,6 +83463,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -83476,14 +83484,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updates to WebAppData renaming "Existing Policies" to "Current Policies"; added contributors to acknowledgement page in docs, updated decarbonization scenario from 0.9 to 0.99 for additional CCS achieved.
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-hongkong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Hong Kong\Models\eps-hongkong\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OutputGraphs!$A$1:$H$131</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$P$528</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29996,7 +29996,7 @@
     <t>**Description:** This policy causes the capital cost of hydrogen vehicles to decline by the set percentage over the course of the model run.  The R&amp;D progress caused by this policy is additional to any R&amp;D necessary to comply with other policies, such as tighter fuel economy standards.  No costs associated with conducting this additional R&amp;D (such as investments in laboratories or engineers' salaries) are included in the model. // **Guidance for setting values:** This policy should generally be set to zero unless you are exploring a scenario with unusual and unexpected technological advancement.  If setting a non-zero value, more mature technologies, such as coal, should have lower values than younger technologies, such as solar.  A setting of 30% implies an average of roughly 1% annual improvement, which is very substantial.</t>
   </si>
   <si>
-    <t>Existing Policies</t>
+    <t>Current Policies</t>
   </si>
 </sst>
 </file>
@@ -31789,9 +31789,6 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -31800,6 +31797,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -32817,7 +32817,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -64428,7 +64428,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30">
+    <row r="30" spans="1:8">
       <c r="A30" s="157" t="s">
         <v>2718</v>
       </c>
@@ -64491,7 +64491,7 @@
       </c>
       <c r="H32" s="156"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="30">
       <c r="A33" s="157" t="s">
         <v>2718</v>
       </c>
@@ -69090,7 +69090,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -81774,13 +81776,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="268" t="s">
+      <c r="A1" s="271" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="268"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="272" t="s">
@@ -81849,13 +81851,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="268" t="s">
+      <c r="A60" s="271" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="268"/>
-      <c r="C60" s="268"/>
-      <c r="D60" s="268"/>
-      <c r="E60" s="268"/>
+      <c r="B60" s="271"/>
+      <c r="C60" s="271"/>
+      <c r="D60" s="271"/>
+      <c r="E60" s="271"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1">
       <c r="A85" s="11" t="s">
@@ -81960,13 +81962,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="268" t="s">
+      <c r="A89" s="271" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="268"/>
-      <c r="C89" s="268"/>
-      <c r="D89" s="268"/>
-      <c r="E89" s="268"/>
+      <c r="B89" s="271"/>
+      <c r="C89" s="271"/>
+      <c r="D89" s="271"/>
+      <c r="E89" s="271"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="11">
@@ -82053,13 +82055,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="268" t="s">
+      <c r="A98" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="268"/>
-      <c r="C98" s="268"/>
-      <c r="D98" s="268"/>
-      <c r="E98" s="268"/>
+      <c r="B98" s="271"/>
+      <c r="C98" s="271"/>
+      <c r="D98" s="271"/>
+      <c r="E98" s="271"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="19">
@@ -82143,13 +82145,13 @@
       <c r="A108" s="22"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="268" t="s">
+      <c r="A109" s="271" t="s">
         <v>187</v>
       </c>
-      <c r="B109" s="268"/>
-      <c r="C109" s="268"/>
-      <c r="D109" s="268"/>
-      <c r="E109" s="268"/>
+      <c r="B109" s="271"/>
+      <c r="C109" s="271"/>
+      <c r="D109" s="271"/>
+      <c r="E109" s="271"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1">
@@ -82162,13 +82164,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="268" t="s">
+      <c r="A113" s="271" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="268"/>
-      <c r="C113" s="268"/>
-      <c r="D113" s="268"/>
-      <c r="E113" s="268"/>
+      <c r="B113" s="271"/>
+      <c r="C113" s="271"/>
+      <c r="D113" s="271"/>
+      <c r="E113" s="271"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="19">
@@ -82249,13 +82251,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="268" t="s">
+      <c r="A124" s="271" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="268"/>
-      <c r="C124" s="268"/>
-      <c r="D124" s="268"/>
-      <c r="E124" s="268"/>
+      <c r="B124" s="271"/>
+      <c r="C124" s="271"/>
+      <c r="D124" s="271"/>
+      <c r="E124" s="271"/>
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:14">
@@ -82346,13 +82348,13 @@
       <c r="C133" s="17"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="268" t="s">
+      <c r="A134" s="271" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="268"/>
-      <c r="C134" s="268"/>
-      <c r="D134" s="268"/>
-      <c r="E134" s="268"/>
+      <c r="B134" s="271"/>
+      <c r="C134" s="271"/>
+      <c r="D134" s="271"/>
+      <c r="E134" s="271"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="29" t="s">
@@ -82367,25 +82369,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75">
       <c r="A136" s="31"/>
-      <c r="B136" s="269" t="s">
+      <c r="B136" s="268" t="s">
         <v>469</v>
       </c>
-      <c r="C136" s="270"/>
-      <c r="D136" s="270"/>
-      <c r="E136" s="271"/>
+      <c r="C136" s="269"/>
+      <c r="D136" s="269"/>
+      <c r="E136" s="270"/>
       <c r="F136" s="30"/>
       <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:14" ht="15.75">
       <c r="A137" s="32"/>
-      <c r="B137" s="269" t="s">
+      <c r="B137" s="268" t="s">
         <v>470</v>
       </c>
-      <c r="C137" s="271"/>
-      <c r="D137" s="269" t="s">
+      <c r="C137" s="270"/>
+      <c r="D137" s="268" t="s">
         <v>471</v>
       </c>
-      <c r="E137" s="271"/>
+      <c r="E137" s="270"/>
       <c r="F137" s="30"/>
       <c r="G137" s="30"/>
     </row>
@@ -82932,13 +82934,13 @@
       <c r="G163" s="30"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="268" t="s">
+      <c r="A165" s="271" t="s">
         <v>190</v>
       </c>
-      <c r="B165" s="268"/>
-      <c r="C165" s="268"/>
-      <c r="D165" s="268"/>
-      <c r="E165" s="268"/>
+      <c r="B165" s="271"/>
+      <c r="C165" s="271"/>
+      <c r="D165" s="271"/>
+      <c r="E165" s="271"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1">
       <c r="A166" s="25" t="s">
@@ -82961,10 +82963,10 @@
       <c r="B168" s="48"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="268" t="s">
+      <c r="A169" s="271" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="268"/>
+      <c r="B169" s="271"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="25" t="s">
@@ -82996,13 +82998,13 @@
       <c r="B173" s="48"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="268" t="s">
+      <c r="A174" s="271" t="s">
         <v>199</v>
       </c>
-      <c r="B174" s="268"/>
-      <c r="C174" s="268"/>
-      <c r="D174" s="268"/>
-      <c r="E174" s="268"/>
+      <c r="B174" s="271"/>
+      <c r="C174" s="271"/>
+      <c r="D174" s="271"/>
+      <c r="E174" s="271"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1">
       <c r="A175" s="25" t="s">
@@ -83022,13 +83024,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="268" t="s">
+      <c r="A178" s="271" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="268"/>
-      <c r="C178" s="268"/>
-      <c r="D178" s="268"/>
-      <c r="E178" s="268"/>
+      <c r="B178" s="271"/>
+      <c r="C178" s="271"/>
+      <c r="D178" s="271"/>
+      <c r="E178" s="271"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="27" t="s">
@@ -83056,13 +83058,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="268" t="s">
+      <c r="A183" s="271" t="s">
         <v>195</v>
       </c>
-      <c r="B183" s="268"/>
-      <c r="C183" s="268"/>
-      <c r="D183" s="268"/>
-      <c r="E183" s="268"/>
+      <c r="B183" s="271"/>
+      <c r="C183" s="271"/>
+      <c r="D183" s="271"/>
+      <c r="E183" s="271"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="25" t="s">
@@ -83117,13 +83119,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="268" t="s">
+      <c r="A191" s="271" t="s">
         <v>209</v>
       </c>
-      <c r="B191" s="268"/>
-      <c r="C191" s="268"/>
-      <c r="D191" s="268"/>
-      <c r="E191" s="268"/>
+      <c r="B191" s="271"/>
+      <c r="C191" s="271"/>
+      <c r="D191" s="271"/>
+      <c r="E191" s="271"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="23" t="s">
@@ -83183,6 +83185,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -83197,12 +83205,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -83211,24 +83213,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -83462,10 +83446,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6678DB7D-994F-458C-B587-D93AD4274EC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -83489,21 +83503,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6678DB7D-994F-458C-B587-D93AD4274EC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
-    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix to baseline scneario name.
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -29996,7 +29996,7 @@
     <t>**Description:** This policy causes the capital cost of hydrogen vehicles to decline by the set percentage over the course of the model run.  The R&amp;D progress caused by this policy is additional to any R&amp;D necessary to comply with other policies, such as tighter fuel economy standards.  No costs associated with conducting this additional R&amp;D (such as investments in laboratories or engineers' salaries) are included in the model. // **Guidance for setting values:** This policy should generally be set to zero unless you are exploring a scenario with unusual and unexpected technological advancement.  If setting a non-zero value, more mature technologies, such as coal, should have lower values than younger technologies, such as solar.  A setting of 30% implies an average of roughly 1% annual improvement, which is very substantial.</t>
   </si>
   <si>
-    <t>Current Policies</t>
+    <t>Current Policy Scenario</t>
   </si>
 </sst>
 </file>
@@ -31789,6 +31789,9 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -31797,9 +31800,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -69091,7 +69091,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -81776,13 +81776,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
+      <c r="B1" s="268"/>
+      <c r="C1" s="268"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="272" t="s">
@@ -81851,13 +81851,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="271" t="s">
+      <c r="A60" s="268" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="271"/>
-      <c r="C60" s="271"/>
-      <c r="D60" s="271"/>
-      <c r="E60" s="271"/>
+      <c r="B60" s="268"/>
+      <c r="C60" s="268"/>
+      <c r="D60" s="268"/>
+      <c r="E60" s="268"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1">
       <c r="A85" s="11" t="s">
@@ -81962,13 +81962,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="271" t="s">
+      <c r="A89" s="268" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="271"/>
-      <c r="C89" s="271"/>
-      <c r="D89" s="271"/>
-      <c r="E89" s="271"/>
+      <c r="B89" s="268"/>
+      <c r="C89" s="268"/>
+      <c r="D89" s="268"/>
+      <c r="E89" s="268"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="11">
@@ -82055,13 +82055,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="271" t="s">
+      <c r="A98" s="268" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="271"/>
-      <c r="C98" s="271"/>
-      <c r="D98" s="271"/>
-      <c r="E98" s="271"/>
+      <c r="B98" s="268"/>
+      <c r="C98" s="268"/>
+      <c r="D98" s="268"/>
+      <c r="E98" s="268"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="19">
@@ -82145,13 +82145,13 @@
       <c r="A108" s="22"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="271" t="s">
+      <c r="A109" s="268" t="s">
         <v>187</v>
       </c>
-      <c r="B109" s="271"/>
-      <c r="C109" s="271"/>
-      <c r="D109" s="271"/>
-      <c r="E109" s="271"/>
+      <c r="B109" s="268"/>
+      <c r="C109" s="268"/>
+      <c r="D109" s="268"/>
+      <c r="E109" s="268"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1">
@@ -82164,13 +82164,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="271" t="s">
+      <c r="A113" s="268" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="271"/>
-      <c r="C113" s="271"/>
-      <c r="D113" s="271"/>
-      <c r="E113" s="271"/>
+      <c r="B113" s="268"/>
+      <c r="C113" s="268"/>
+      <c r="D113" s="268"/>
+      <c r="E113" s="268"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="19">
@@ -82251,13 +82251,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="271" t="s">
+      <c r="A124" s="268" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="271"/>
-      <c r="C124" s="271"/>
-      <c r="D124" s="271"/>
-      <c r="E124" s="271"/>
+      <c r="B124" s="268"/>
+      <c r="C124" s="268"/>
+      <c r="D124" s="268"/>
+      <c r="E124" s="268"/>
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:14">
@@ -82348,13 +82348,13 @@
       <c r="C133" s="17"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="271" t="s">
+      <c r="A134" s="268" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="271"/>
-      <c r="C134" s="271"/>
-      <c r="D134" s="271"/>
-      <c r="E134" s="271"/>
+      <c r="B134" s="268"/>
+      <c r="C134" s="268"/>
+      <c r="D134" s="268"/>
+      <c r="E134" s="268"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="29" t="s">
@@ -82369,25 +82369,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75">
       <c r="A136" s="31"/>
-      <c r="B136" s="268" t="s">
+      <c r="B136" s="269" t="s">
         <v>469</v>
       </c>
-      <c r="C136" s="269"/>
-      <c r="D136" s="269"/>
-      <c r="E136" s="270"/>
+      <c r="C136" s="270"/>
+      <c r="D136" s="270"/>
+      <c r="E136" s="271"/>
       <c r="F136" s="30"/>
       <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:14" ht="15.75">
       <c r="A137" s="32"/>
-      <c r="B137" s="268" t="s">
+      <c r="B137" s="269" t="s">
         <v>470</v>
       </c>
-      <c r="C137" s="270"/>
-      <c r="D137" s="268" t="s">
+      <c r="C137" s="271"/>
+      <c r="D137" s="269" t="s">
         <v>471</v>
       </c>
-      <c r="E137" s="270"/>
+      <c r="E137" s="271"/>
       <c r="F137" s="30"/>
       <c r="G137" s="30"/>
     </row>
@@ -82934,13 +82934,13 @@
       <c r="G163" s="30"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="271" t="s">
+      <c r="A165" s="268" t="s">
         <v>190</v>
       </c>
-      <c r="B165" s="271"/>
-      <c r="C165" s="271"/>
-      <c r="D165" s="271"/>
-      <c r="E165" s="271"/>
+      <c r="B165" s="268"/>
+      <c r="C165" s="268"/>
+      <c r="D165" s="268"/>
+      <c r="E165" s="268"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1">
       <c r="A166" s="25" t="s">
@@ -82963,10 +82963,10 @@
       <c r="B168" s="48"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="271" t="s">
+      <c r="A169" s="268" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="271"/>
+      <c r="B169" s="268"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="25" t="s">
@@ -82998,13 +82998,13 @@
       <c r="B173" s="48"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="271" t="s">
+      <c r="A174" s="268" t="s">
         <v>199</v>
       </c>
-      <c r="B174" s="271"/>
-      <c r="C174" s="271"/>
-      <c r="D174" s="271"/>
-      <c r="E174" s="271"/>
+      <c r="B174" s="268"/>
+      <c r="C174" s="268"/>
+      <c r="D174" s="268"/>
+      <c r="E174" s="268"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1">
       <c r="A175" s="25" t="s">
@@ -83024,13 +83024,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="271" t="s">
+      <c r="A178" s="268" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="271"/>
-      <c r="C178" s="271"/>
-      <c r="D178" s="271"/>
-      <c r="E178" s="271"/>
+      <c r="B178" s="268"/>
+      <c r="C178" s="268"/>
+      <c r="D178" s="268"/>
+      <c r="E178" s="268"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="27" t="s">
@@ -83058,13 +83058,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="271" t="s">
+      <c r="A183" s="268" t="s">
         <v>195</v>
       </c>
-      <c r="B183" s="271"/>
-      <c r="C183" s="271"/>
-      <c r="D183" s="271"/>
-      <c r="E183" s="271"/>
+      <c r="B183" s="268"/>
+      <c r="C183" s="268"/>
+      <c r="D183" s="268"/>
+      <c r="E183" s="268"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="25" t="s">
@@ -83119,13 +83119,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="271" t="s">
+      <c r="A191" s="268" t="s">
         <v>209</v>
       </c>
-      <c r="B191" s="271"/>
-      <c r="C191" s="271"/>
-      <c r="D191" s="271"/>
-      <c r="E191" s="271"/>
+      <c r="B191" s="268"/>
+      <c r="C191" s="268"/>
+      <c r="D191" s="268"/>
+      <c r="E191" s="268"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="23" t="s">
@@ -83185,12 +83185,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -83205,6 +83199,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -83213,6 +83213,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -83446,15 +83455,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -83465,6 +83465,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6678DB7D-994F-458C-B587-D93AD4274EC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -83484,24 +83502,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update name for decarb scenario
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Hong Kong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06576AEF-806E-49EA-8DF3-E1F55A615635}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476142C-AEF9-4314-86C5-DEF6EB7D09B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10350" yWindow="615" windowWidth="17805" windowHeight="16695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="360" windowWidth="17805" windowHeight="16695" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -29890,9 +29890,6 @@
     <t>2018 HKD / barrel</t>
   </si>
   <si>
-    <t>Scenario_Decarbonization.cin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of EV chargers: https://www.epd.gov.hk/epd/english/environmentinhk/air/prob_solutions/promotion_ev.html                                   </t>
   </si>
   <si>
@@ -30023,6 +30020,9 @@
   </si>
   <si>
     <t>indst cropland and rice measures</t>
+  </si>
+  <si>
+    <t>Senario_Decarbonization.cin</t>
   </si>
 </sst>
 </file>
@@ -31830,6 +31830,9 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -31838,9 +31841,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -32967,7 +32967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T553"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K2" sqref="K2"/>
     </sheetView>
@@ -36586,7 +36586,7 @@
         <v>2635</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="T62" s="3">
         <v>0</v>
@@ -36644,7 +36644,7 @@
         <v>2636</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="T63" s="3">
         <v>0</v>
@@ -37352,7 +37352,7 @@
         <v>93</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="H75" s="57">
         <v>518</v>
@@ -37379,7 +37379,7 @@
         <v>537</v>
       </c>
       <c r="P75" s="3" t="s">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="Q75" s="3" t="s">
         <v>538</v>
@@ -38140,7 +38140,7 @@
         <v>122</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="Q89" s="3" t="s">
         <v>217</v>
@@ -38202,7 +38202,7 @@
         <v>122</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="Q90" s="3" t="s">
         <v>217</v>
@@ -38264,7 +38264,7 @@
         <v>122</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="Q91" s="3" t="s">
         <v>217</v>
@@ -38326,7 +38326,7 @@
         <v>122</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>217</v>
@@ -38574,7 +38574,7 @@
         <v>122</v>
       </c>
       <c r="P96" s="3" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="Q96" s="3" t="s">
         <v>217</v>
@@ -38698,7 +38698,7 @@
         <v>122</v>
       </c>
       <c r="P98" s="3" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="Q98" s="3" t="s">
         <v>217</v>
@@ -38822,7 +38822,7 @@
         <v>122</v>
       </c>
       <c r="P100" s="3" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="Q100" s="3" t="s">
         <v>217</v>
@@ -47841,7 +47841,7 @@
         <v>19</v>
       </c>
       <c r="K267" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L267" s="65"/>
       <c r="M267" s="65"/>
@@ -47893,7 +47893,7 @@
         <v>19</v>
       </c>
       <c r="K268" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L268" s="66"/>
       <c r="M268" s="66"/>
@@ -47945,7 +47945,7 @@
         <v>19</v>
       </c>
       <c r="K269" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L269" s="67">
         <v>0</v>
@@ -48003,7 +48003,7 @@
         <v>19</v>
       </c>
       <c r="K270" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L270" s="66"/>
       <c r="M270" s="66"/>
@@ -48055,7 +48055,7 @@
         <v>19</v>
       </c>
       <c r="K271" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L271" s="66">
         <v>0</v>
@@ -48115,7 +48115,7 @@
         <v>19</v>
       </c>
       <c r="K272" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L272" s="66">
         <v>0</v>
@@ -48175,7 +48175,7 @@
         <v>19</v>
       </c>
       <c r="K273" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L273" s="66">
         <v>0</v>
@@ -48235,7 +48235,7 @@
         <v>19</v>
       </c>
       <c r="K274" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L274" s="66">
         <v>0</v>
@@ -48293,7 +48293,7 @@
         <v>19</v>
       </c>
       <c r="K275" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L275" s="64"/>
       <c r="M275" s="64"/>
@@ -48345,7 +48345,7 @@
         <v>19</v>
       </c>
       <c r="K276" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L276" s="66">
         <v>0</v>
@@ -48403,7 +48403,7 @@
         <v>19</v>
       </c>
       <c r="K277" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L277" s="66"/>
       <c r="M277" s="66"/>
@@ -48453,7 +48453,7 @@
         <v>19</v>
       </c>
       <c r="K278" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L278" s="66"/>
       <c r="M278" s="66"/>
@@ -48503,7 +48503,7 @@
         <v>19</v>
       </c>
       <c r="K279" s="155" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="L279" s="66"/>
       <c r="M279" s="66"/>
@@ -48553,7 +48553,7 @@
         <v>23</v>
       </c>
       <c r="K280" s="156" t="s">
-        <v>3014</v>
+        <v>3013</v>
       </c>
       <c r="L280" s="59">
         <v>0</v>
@@ -54641,7 +54641,7 @@
         <v>405</v>
       </c>
       <c r="K379" s="156" t="s">
-        <v>3013</v>
+        <v>3012</v>
       </c>
       <c r="L379" s="59">
         <v>0</v>
@@ -55499,7 +55499,7 @@
         <v>155</v>
       </c>
       <c r="K394" s="155" t="s">
-        <v>3015</v>
+        <v>3014</v>
       </c>
       <c r="L394" s="59">
         <v>0</v>
@@ -55723,7 +55723,7 @@
         <v>156</v>
       </c>
       <c r="K398" s="155" t="s">
-        <v>3015</v>
+        <v>3014</v>
       </c>
       <c r="L398" s="59">
         <v>0</v>
@@ -61364,7 +61364,7 @@
       </c>
       <c r="E500" s="54"/>
       <c r="F500" s="3" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="G500" s="3" t="s">
         <v>213</v>
@@ -61394,7 +61394,7 @@
         <v>37</v>
       </c>
       <c r="P500" s="3" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="Q500" s="3" t="s">
         <v>283</v>
@@ -61424,7 +61424,7 @@
       </c>
       <c r="E501" s="54"/>
       <c r="F501" s="3" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="G501" s="3"/>
       <c r="H501" s="55">
@@ -61452,7 +61452,7 @@
         <v>37</v>
       </c>
       <c r="P501" s="3" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="Q501" s="3" t="s">
         <v>283</v>
@@ -63284,7 +63284,7 @@
       </c>
       <c r="E533" s="54"/>
       <c r="F533" s="3" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="G533" s="3" t="s">
         <v>213</v>
@@ -63314,7 +63314,7 @@
         <v>38</v>
       </c>
       <c r="P533" s="3" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="Q533" s="3" t="s">
         <v>283</v>
@@ -63343,7 +63343,7 @@
         <v>2424</v>
       </c>
       <c r="F534" s="5" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="H534" s="237">
         <v>519</v>
@@ -63370,7 +63370,7 @@
         <v>38</v>
       </c>
       <c r="P534" s="3" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="Q534" s="3" t="s">
         <v>283</v>
@@ -63782,7 +63782,7 @@
         <v>2113</v>
       </c>
       <c r="C1" s="255" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="D1" s="231" t="s">
         <v>68</v>
@@ -63803,34 +63803,34 @@
         <v>350</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>3001</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>3002</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3003</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>3004</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3005</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3006</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3007</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3008</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>3009</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>3010</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3011</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -64570,7 +64570,7 @@
         <v>71</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F30" s="162" t="s">
         <v>416</v>
@@ -64594,7 +64594,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F31" s="162" t="s">
         <v>416</v>
@@ -64618,7 +64618,7 @@
         <v>71</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F32" s="162" t="s">
         <v>416</v>
@@ -64642,7 +64642,7 @@
         <v>71</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F33" s="162" t="s">
         <v>416</v>
@@ -64666,7 +64666,7 @@
         <v>71</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F34" s="162" t="s">
         <v>416</v>
@@ -64676,7 +64676,7 @@
       </c>
       <c r="I34" s="156"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="157" t="s">
         <v>2703</v>
       </c>
@@ -64690,7 +64690,7 @@
         <v>71</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F35" s="162" t="s">
         <v>416</v>
@@ -64714,7 +64714,7 @@
         <v>71</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="F36" s="224" t="s">
         <v>416</v>
@@ -65546,7 +65546,7 @@
         <v>74</v>
       </c>
       <c r="F66" s="156" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="G66" s="157" t="s">
         <v>2930</v>
@@ -65575,7 +65575,7 @@
         <v>74</v>
       </c>
       <c r="F67" s="196" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="G67" s="196" t="s">
         <v>2911</v>
@@ -65981,7 +65981,7 @@
         <v>74</v>
       </c>
       <c r="F81" s="157" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="G81" s="157" t="s">
         <v>2914</v>
@@ -66010,7 +66010,7 @@
         <v>74</v>
       </c>
       <c r="F82" s="157" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="G82" s="195" t="s">
         <v>2934</v>
@@ -66039,7 +66039,7 @@
         <v>74</v>
       </c>
       <c r="F83" s="157" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="G83" s="156" t="s">
         <v>2519</v>
@@ -66068,7 +66068,7 @@
         <v>74</v>
       </c>
       <c r="F84" s="157" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="G84" s="156" t="s">
         <v>2704</v>
@@ -66097,7 +66097,7 @@
         <v>74</v>
       </c>
       <c r="F85" s="157" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="G85" s="156" t="s">
         <v>2711</v>
@@ -66126,7 +66126,7 @@
         <v>74</v>
       </c>
       <c r="F86" s="195" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G86" s="196" t="s">
         <v>2712</v>
@@ -66271,7 +66271,7 @@
         <v>74</v>
       </c>
       <c r="F91" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G91" s="157" t="s">
         <v>2940</v>
@@ -66300,7 +66300,7 @@
         <v>74</v>
       </c>
       <c r="F92" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G92" s="157" t="s">
         <v>2202</v>
@@ -66329,7 +66329,7 @@
         <v>74</v>
       </c>
       <c r="F93" s="253" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G93" s="195" t="s">
         <v>2945</v>
@@ -66358,7 +66358,7 @@
         <v>74</v>
       </c>
       <c r="F94" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G94" s="157" t="s">
         <v>2946</v>
@@ -66387,7 +66387,7 @@
         <v>74</v>
       </c>
       <c r="F95" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G95" s="157" t="s">
         <v>2918</v>
@@ -66416,7 +66416,7 @@
         <v>72</v>
       </c>
       <c r="F96" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G96" s="156" t="s">
         <v>2118</v>
@@ -66440,7 +66440,7 @@
         <v>72</v>
       </c>
       <c r="F97" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G97" s="156" t="s">
         <v>2117</v>
@@ -66464,7 +66464,7 @@
         <v>72</v>
       </c>
       <c r="F98" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G98" s="156" t="s">
         <v>2116</v>
@@ -66488,7 +66488,7 @@
         <v>72</v>
       </c>
       <c r="F99" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G99" s="156" t="s">
         <v>2115</v>
@@ -66512,7 +66512,7 @@
         <v>72</v>
       </c>
       <c r="F100" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G100" s="156" t="s">
         <v>2114</v>
@@ -66536,7 +66536,7 @@
         <v>72</v>
       </c>
       <c r="F101" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G101" s="156" t="s">
         <v>2190</v>
@@ -66560,7 +66560,7 @@
         <v>72</v>
       </c>
       <c r="F102" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G102" s="156" t="s">
         <v>2191</v>
@@ -66584,7 +66584,7 @@
         <v>72</v>
       </c>
       <c r="F103" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G103" s="156" t="s">
         <v>2549</v>
@@ -66608,7 +66608,7 @@
         <v>72</v>
       </c>
       <c r="F104" s="252" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G104" s="156" t="s">
         <v>2550</v>
@@ -66657,7 +66657,7 @@
         <v>74</v>
       </c>
       <c r="F106" s="254" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G106" s="156" t="s">
         <v>2562</v>
@@ -66686,7 +66686,7 @@
         <v>72</v>
       </c>
       <c r="F107" s="254" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G107" s="156" t="s">
         <v>2565</v>
@@ -66773,7 +66773,7 @@
         <v>74</v>
       </c>
       <c r="F110" s="254" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G110" s="156" t="s">
         <v>2699</v>
@@ -66802,7 +66802,7 @@
         <v>72</v>
       </c>
       <c r="F111" s="254" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G111" s="156" t="s">
         <v>2700</v>
@@ -66889,7 +66889,7 @@
         <v>74</v>
       </c>
       <c r="F114" s="254" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G114" s="156" t="s">
         <v>2742</v>
@@ -66918,7 +66918,7 @@
         <v>72</v>
       </c>
       <c r="F115" s="254" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G115" s="196" t="s">
         <v>2743</v>
@@ -66976,7 +66976,7 @@
         <v>2181</v>
       </c>
       <c r="F117" s="252" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="G117" s="156" t="s">
         <v>2579</v>
@@ -67005,7 +67005,7 @@
         <v>2181</v>
       </c>
       <c r="F118" s="252" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="G118" s="156" t="s">
         <v>2193</v>
@@ -67034,7 +67034,7 @@
         <v>2181</v>
       </c>
       <c r="F119" s="252" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="G119" s="156" t="s">
         <v>2571</v>
@@ -67063,7 +67063,7 @@
         <v>2181</v>
       </c>
       <c r="F120" s="252" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="G120" s="156" t="s">
         <v>2195</v>
@@ -67092,7 +67092,7 @@
         <v>2181</v>
       </c>
       <c r="F121" s="252" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="G121" s="156" t="s">
         <v>2574</v>
@@ -67121,7 +67121,7 @@
         <v>2181</v>
       </c>
       <c r="F122" s="252" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="G122" s="156" t="s">
         <v>2575</v>
@@ -67179,7 +67179,7 @@
         <v>2181</v>
       </c>
       <c r="F124" s="252" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="G124" s="156" t="s">
         <v>2582</v>
@@ -69532,7 +69532,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -69553,10 +69553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="228" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="B2" s="228" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -69564,7 +69564,7 @@
         <v>2961</v>
       </c>
       <c r="B3" s="228" t="s">
-        <v>2971</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -82218,13 +82218,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="274" t="s">
+      <c r="A1" s="271" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="274"/>
-      <c r="C1" s="274"/>
-      <c r="D1" s="274"/>
-      <c r="E1" s="274"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="275" t="s">
@@ -82293,13 +82293,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="274" t="s">
+      <c r="A60" s="271" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="274"/>
-      <c r="C60" s="274"/>
-      <c r="D60" s="274"/>
-      <c r="E60" s="274"/>
+      <c r="B60" s="271"/>
+      <c r="C60" s="271"/>
+      <c r="D60" s="271"/>
+      <c r="E60" s="271"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
@@ -82404,13 +82404,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A89" s="274" t="s">
+      <c r="A89" s="271" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="274"/>
-      <c r="C89" s="274"/>
-      <c r="D89" s="274"/>
-      <c r="E89" s="274"/>
+      <c r="B89" s="271"/>
+      <c r="C89" s="271"/>
+      <c r="D89" s="271"/>
+      <c r="E89" s="271"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
@@ -82497,13 +82497,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="274" t="s">
+      <c r="A98" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="274"/>
-      <c r="C98" s="274"/>
-      <c r="D98" s="274"/>
-      <c r="E98" s="274"/>
+      <c r="B98" s="271"/>
+      <c r="C98" s="271"/>
+      <c r="D98" s="271"/>
+      <c r="E98" s="271"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="19">
@@ -82587,13 +82587,13 @@
       <c r="A108" s="22"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="274" t="s">
+      <c r="A109" s="271" t="s">
         <v>187</v>
       </c>
-      <c r="B109" s="274"/>
-      <c r="C109" s="274"/>
-      <c r="D109" s="274"/>
-      <c r="E109" s="274"/>
+      <c r="B109" s="271"/>
+      <c r="C109" s="271"/>
+      <c r="D109" s="271"/>
+      <c r="E109" s="271"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -82606,13 +82606,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A113" s="274" t="s">
+      <c r="A113" s="271" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="274"/>
-      <c r="C113" s="274"/>
-      <c r="D113" s="274"/>
-      <c r="E113" s="274"/>
+      <c r="B113" s="271"/>
+      <c r="C113" s="271"/>
+      <c r="D113" s="271"/>
+      <c r="E113" s="271"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="19">
@@ -82693,13 +82693,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A124" s="274" t="s">
+      <c r="A124" s="271" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="274"/>
-      <c r="C124" s="274"/>
-      <c r="D124" s="274"/>
-      <c r="E124" s="274"/>
+      <c r="B124" s="271"/>
+      <c r="C124" s="271"/>
+      <c r="D124" s="271"/>
+      <c r="E124" s="271"/>
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -82790,13 +82790,13 @@
       <c r="C133" s="17"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A134" s="274" t="s">
+      <c r="A134" s="271" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="274"/>
-      <c r="C134" s="274"/>
-      <c r="D134" s="274"/>
-      <c r="E134" s="274"/>
+      <c r="B134" s="271"/>
+      <c r="C134" s="271"/>
+      <c r="D134" s="271"/>
+      <c r="E134" s="271"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="29" t="s">
@@ -82811,25 +82811,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A136" s="31"/>
-      <c r="B136" s="271" t="s">
+      <c r="B136" s="272" t="s">
         <v>469</v>
       </c>
-      <c r="C136" s="272"/>
-      <c r="D136" s="272"/>
-      <c r="E136" s="273"/>
+      <c r="C136" s="273"/>
+      <c r="D136" s="273"/>
+      <c r="E136" s="274"/>
       <c r="F136" s="30"/>
       <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A137" s="32"/>
-      <c r="B137" s="271" t="s">
+      <c r="B137" s="272" t="s">
         <v>470</v>
       </c>
-      <c r="C137" s="273"/>
-      <c r="D137" s="271" t="s">
+      <c r="C137" s="274"/>
+      <c r="D137" s="272" t="s">
         <v>471</v>
       </c>
-      <c r="E137" s="273"/>
+      <c r="E137" s="274"/>
       <c r="F137" s="30"/>
       <c r="G137" s="30"/>
     </row>
@@ -83376,13 +83376,13 @@
       <c r="G163" s="30"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="274" t="s">
+      <c r="A165" s="271" t="s">
         <v>190</v>
       </c>
-      <c r="B165" s="274"/>
-      <c r="C165" s="274"/>
-      <c r="D165" s="274"/>
-      <c r="E165" s="274"/>
+      <c r="B165" s="271"/>
+      <c r="C165" s="271"/>
+      <c r="D165" s="271"/>
+      <c r="E165" s="271"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="25" t="s">
@@ -83405,10 +83405,10 @@
       <c r="B168" s="48"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="274" t="s">
+      <c r="A169" s="271" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="274"/>
+      <c r="B169" s="271"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="25" t="s">
@@ -83440,13 +83440,13 @@
       <c r="B173" s="48"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="274" t="s">
+      <c r="A174" s="271" t="s">
         <v>199</v>
       </c>
-      <c r="B174" s="274"/>
-      <c r="C174" s="274"/>
-      <c r="D174" s="274"/>
-      <c r="E174" s="274"/>
+      <c r="B174" s="271"/>
+      <c r="C174" s="271"/>
+      <c r="D174" s="271"/>
+      <c r="E174" s="271"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="25" t="s">
@@ -83466,13 +83466,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="274" t="s">
+      <c r="A178" s="271" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="274"/>
-      <c r="C178" s="274"/>
-      <c r="D178" s="274"/>
-      <c r="E178" s="274"/>
+      <c r="B178" s="271"/>
+      <c r="C178" s="271"/>
+      <c r="D178" s="271"/>
+      <c r="E178" s="271"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="27" t="s">
@@ -83500,13 +83500,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="274" t="s">
+      <c r="A183" s="271" t="s">
         <v>195</v>
       </c>
-      <c r="B183" s="274"/>
-      <c r="C183" s="274"/>
-      <c r="D183" s="274"/>
-      <c r="E183" s="274"/>
+      <c r="B183" s="271"/>
+      <c r="C183" s="271"/>
+      <c r="D183" s="271"/>
+      <c r="E183" s="271"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
@@ -83561,13 +83561,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="274" t="s">
+      <c r="A191" s="271" t="s">
         <v>209</v>
       </c>
-      <c r="B191" s="274"/>
-      <c r="C191" s="274"/>
-      <c r="D191" s="274"/>
-      <c r="E191" s="274"/>
+      <c r="B191" s="271"/>
+      <c r="C191" s="271"/>
+      <c r="D191" s="271"/>
+      <c r="E191" s="271"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="23" t="s">
@@ -83627,12 +83627,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -83647,6 +83641,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -83655,21 +83655,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005D5DE895D8AE54A972C2171818FD093" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85f6924c4aafd897c3f23384ae9dc35">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01f24951-2a3e-4fd5-a813-71a74687f653" xmlns:ns3="80a27e12-bb1f-4e28-b766-51f62aa5c67e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11afb4ea5aef950dd888cd3ab39ccec1" ns2:_="" ns3:_="">
     <xsd:import namespace="01f24951-2a3e-4fd5-a813-71a74687f653"/>
@@ -83886,33 +83871,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B682BFB-0987-4DD0-9AC2-B04E7019F68C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -83929,4 +83903,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update policy sched names
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Hong Kong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476142C-AEF9-4314-86C5-DEF6EB7D09B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDC1DDD-882E-49BF-9F23-44697CA5C68C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="360" windowWidth="17805" windowHeight="16695" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="3570" windowWidth="17745" windowHeight="13890" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -470,7 +470,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11057" uniqueCount="3016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11057" uniqueCount="3017">
   <si>
     <t>Short Name</t>
   </si>
@@ -30010,19 +30010,22 @@
     <t>Target 2 Description</t>
   </si>
   <si>
-    <t>elec generation subsidy</t>
-  </si>
-  <si>
-    <t>indst f gas substitution</t>
-  </si>
-  <si>
-    <t>indst cement measures</t>
-  </si>
-  <si>
-    <t>indst cropland and rice measures</t>
-  </si>
-  <si>
     <t>Senario_Decarbonization.cin</t>
+  </si>
+  <si>
+    <t>elec subsidy</t>
+  </si>
+  <si>
+    <t>indst cement clinker substitution</t>
+  </si>
+  <si>
+    <t>indst avoid F gases</t>
+  </si>
+  <si>
+    <t>indst rice cultivation measures</t>
+  </si>
+  <si>
+    <t>indst cropland management</t>
   </si>
 </sst>
 </file>
@@ -31830,9 +31833,6 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -31841,6 +31841,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -32967,9 +32970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T553"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47841,7 +47844,7 @@
         <v>19</v>
       </c>
       <c r="K267" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L267" s="65"/>
       <c r="M267" s="65"/>
@@ -47893,7 +47896,7 @@
         <v>19</v>
       </c>
       <c r="K268" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L268" s="66"/>
       <c r="M268" s="66"/>
@@ -47945,7 +47948,7 @@
         <v>19</v>
       </c>
       <c r="K269" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L269" s="67">
         <v>0</v>
@@ -48003,7 +48006,7 @@
         <v>19</v>
       </c>
       <c r="K270" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L270" s="66"/>
       <c r="M270" s="66"/>
@@ -48055,7 +48058,7 @@
         <v>19</v>
       </c>
       <c r="K271" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L271" s="66">
         <v>0</v>
@@ -48115,7 +48118,7 @@
         <v>19</v>
       </c>
       <c r="K272" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L272" s="66">
         <v>0</v>
@@ -48175,7 +48178,7 @@
         <v>19</v>
       </c>
       <c r="K273" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L273" s="66">
         <v>0</v>
@@ -48235,7 +48238,7 @@
         <v>19</v>
       </c>
       <c r="K274" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L274" s="66">
         <v>0</v>
@@ -48293,7 +48296,7 @@
         <v>19</v>
       </c>
       <c r="K275" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L275" s="64"/>
       <c r="M275" s="64"/>
@@ -48345,7 +48348,7 @@
         <v>19</v>
       </c>
       <c r="K276" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L276" s="66">
         <v>0</v>
@@ -48403,7 +48406,7 @@
         <v>19</v>
       </c>
       <c r="K277" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L277" s="66"/>
       <c r="M277" s="66"/>
@@ -48453,7 +48456,7 @@
         <v>19</v>
       </c>
       <c r="K278" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L278" s="66"/>
       <c r="M278" s="66"/>
@@ -48503,7 +48506,7 @@
         <v>19</v>
       </c>
       <c r="K279" s="155" t="s">
-        <v>3011</v>
+        <v>3012</v>
       </c>
       <c r="L279" s="66"/>
       <c r="M279" s="66"/>
@@ -54641,7 +54644,7 @@
         <v>405</v>
       </c>
       <c r="K379" s="156" t="s">
-        <v>3012</v>
+        <v>3014</v>
       </c>
       <c r="L379" s="59">
         <v>0</v>
@@ -55499,7 +55502,7 @@
         <v>155</v>
       </c>
       <c r="K394" s="155" t="s">
-        <v>3014</v>
+        <v>3016</v>
       </c>
       <c r="L394" s="59">
         <v>0</v>
@@ -55723,7 +55726,7 @@
         <v>156</v>
       </c>
       <c r="K398" s="155" t="s">
-        <v>3014</v>
+        <v>3015</v>
       </c>
       <c r="L398" s="59">
         <v>0</v>
@@ -63519,7 +63522,6 @@
       <c r="S553" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T534" xr:uid="{DC707719-781A-4FB8-B85F-F4D232047DE3}"/>
   <conditionalFormatting sqref="I76:I88 I518 I520:I539 I541:I1048576 I90:I99 I1:I9 I12:I19 I24 I33:I36 I43:I46 I53:I59 I38:I39 I48:I49 I63:I64 I312:I317 I322:I327 I332:I337 I352:I353 I362:I367 I342:I350 I355 I357 I113:I307 I372:I483 I485:I516">
     <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I1)))</formula>
@@ -64700,7 +64702,7 @@
       </c>
       <c r="I35" s="156"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="195" t="s">
         <v>2703</v>
       </c>
@@ -69532,7 +69534,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -69564,7 +69566,7 @@
         <v>2961</v>
       </c>
       <c r="B3" s="228" t="s">
-        <v>3015</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -82218,13 +82220,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="274" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="275" t="s">
@@ -82293,13 +82295,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="271" t="s">
+      <c r="A60" s="274" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="271"/>
-      <c r="C60" s="271"/>
-      <c r="D60" s="271"/>
-      <c r="E60" s="271"/>
+      <c r="B60" s="274"/>
+      <c r="C60" s="274"/>
+      <c r="D60" s="274"/>
+      <c r="E60" s="274"/>
     </row>
     <row r="85" spans="1:39" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
@@ -82404,13 +82406,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A89" s="271" t="s">
+      <c r="A89" s="274" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="271"/>
-      <c r="C89" s="271"/>
-      <c r="D89" s="271"/>
-      <c r="E89" s="271"/>
+      <c r="B89" s="274"/>
+      <c r="C89" s="274"/>
+      <c r="D89" s="274"/>
+      <c r="E89" s="274"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
@@ -82497,13 +82499,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="271" t="s">
+      <c r="A98" s="274" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="271"/>
-      <c r="C98" s="271"/>
-      <c r="D98" s="271"/>
-      <c r="E98" s="271"/>
+      <c r="B98" s="274"/>
+      <c r="C98" s="274"/>
+      <c r="D98" s="274"/>
+      <c r="E98" s="274"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="19">
@@ -82587,13 +82589,13 @@
       <c r="A108" s="22"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="271" t="s">
+      <c r="A109" s="274" t="s">
         <v>187</v>
       </c>
-      <c r="B109" s="271"/>
-      <c r="C109" s="271"/>
-      <c r="D109" s="271"/>
-      <c r="E109" s="271"/>
+      <c r="B109" s="274"/>
+      <c r="C109" s="274"/>
+      <c r="D109" s="274"/>
+      <c r="E109" s="274"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -82606,13 +82608,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A113" s="271" t="s">
+      <c r="A113" s="274" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="271"/>
-      <c r="C113" s="271"/>
-      <c r="D113" s="271"/>
-      <c r="E113" s="271"/>
+      <c r="B113" s="274"/>
+      <c r="C113" s="274"/>
+      <c r="D113" s="274"/>
+      <c r="E113" s="274"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="19">
@@ -82693,13 +82695,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A124" s="271" t="s">
+      <c r="A124" s="274" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="271"/>
-      <c r="C124" s="271"/>
-      <c r="D124" s="271"/>
-      <c r="E124" s="271"/>
+      <c r="B124" s="274"/>
+      <c r="C124" s="274"/>
+      <c r="D124" s="274"/>
+      <c r="E124" s="274"/>
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -82790,13 +82792,13 @@
       <c r="C133" s="17"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A134" s="271" t="s">
+      <c r="A134" s="274" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="271"/>
-      <c r="C134" s="271"/>
-      <c r="D134" s="271"/>
-      <c r="E134" s="271"/>
+      <c r="B134" s="274"/>
+      <c r="C134" s="274"/>
+      <c r="D134" s="274"/>
+      <c r="E134" s="274"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="29" t="s">
@@ -82811,25 +82813,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A136" s="31"/>
-      <c r="B136" s="272" t="s">
+      <c r="B136" s="271" t="s">
         <v>469</v>
       </c>
-      <c r="C136" s="273"/>
-      <c r="D136" s="273"/>
-      <c r="E136" s="274"/>
+      <c r="C136" s="272"/>
+      <c r="D136" s="272"/>
+      <c r="E136" s="273"/>
       <c r="F136" s="30"/>
       <c r="G136" s="30"/>
     </row>
     <row r="137" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A137" s="32"/>
-      <c r="B137" s="272" t="s">
+      <c r="B137" s="271" t="s">
         <v>470</v>
       </c>
-      <c r="C137" s="274"/>
-      <c r="D137" s="272" t="s">
+      <c r="C137" s="273"/>
+      <c r="D137" s="271" t="s">
         <v>471</v>
       </c>
-      <c r="E137" s="274"/>
+      <c r="E137" s="273"/>
       <c r="F137" s="30"/>
       <c r="G137" s="30"/>
     </row>
@@ -83376,13 +83378,13 @@
       <c r="G163" s="30"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="271" t="s">
+      <c r="A165" s="274" t="s">
         <v>190</v>
       </c>
-      <c r="B165" s="271"/>
-      <c r="C165" s="271"/>
-      <c r="D165" s="271"/>
-      <c r="E165" s="271"/>
+      <c r="B165" s="274"/>
+      <c r="C165" s="274"/>
+      <c r="D165" s="274"/>
+      <c r="E165" s="274"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="25" t="s">
@@ -83405,10 +83407,10 @@
       <c r="B168" s="48"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="271" t="s">
+      <c r="A169" s="274" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="271"/>
+      <c r="B169" s="274"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="25" t="s">
@@ -83440,13 +83442,13 @@
       <c r="B173" s="48"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="271" t="s">
+      <c r="A174" s="274" t="s">
         <v>199</v>
       </c>
-      <c r="B174" s="271"/>
-      <c r="C174" s="271"/>
-      <c r="D174" s="271"/>
-      <c r="E174" s="271"/>
+      <c r="B174" s="274"/>
+      <c r="C174" s="274"/>
+      <c r="D174" s="274"/>
+      <c r="E174" s="274"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="25" t="s">
@@ -83466,13 +83468,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="271" t="s">
+      <c r="A178" s="274" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="271"/>
-      <c r="C178" s="271"/>
-      <c r="D178" s="271"/>
-      <c r="E178" s="271"/>
+      <c r="B178" s="274"/>
+      <c r="C178" s="274"/>
+      <c r="D178" s="274"/>
+      <c r="E178" s="274"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="27" t="s">
@@ -83500,13 +83502,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="271" t="s">
+      <c r="A183" s="274" t="s">
         <v>195</v>
       </c>
-      <c r="B183" s="271"/>
-      <c r="C183" s="271"/>
-      <c r="D183" s="271"/>
-      <c r="E183" s="271"/>
+      <c r="B183" s="274"/>
+      <c r="C183" s="274"/>
+      <c r="D183" s="274"/>
+      <c r="E183" s="274"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
@@ -83561,13 +83563,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="271" t="s">
+      <c r="A191" s="274" t="s">
         <v>209</v>
       </c>
-      <c r="B191" s="271"/>
-      <c r="C191" s="271"/>
-      <c r="D191" s="271"/>
-      <c r="E191" s="271"/>
+      <c r="B191" s="274"/>
+      <c r="C191" s="274"/>
+      <c r="D191" s="274"/>
+      <c r="E191" s="274"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="23" t="s">
@@ -83627,6 +83629,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -83641,12 +83649,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -83655,6 +83657,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005D5DE895D8AE54A972C2171818FD093" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85f6924c4aafd897c3f23384ae9dc35">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01f24951-2a3e-4fd5-a813-71a74687f653" xmlns:ns3="80a27e12-bb1f-4e28-b766-51f62aa5c67e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11afb4ea5aef950dd888cd3ab39ccec1" ns2:_="" ns3:_="">
     <xsd:import namespace="01f24951-2a3e-4fd5-a813-71a74687f653"/>
@@ -83871,22 +83888,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B682BFB-0987-4DD0-9AC2-B04E7019F68C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -83903,30 +83931,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21ECD4D-B929-45FA-9AAA-1B0FF4AB87F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79E02BA-2700-422F-BE0F-6DD1255557BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>